<commit_message>
Update to the new CubeMX version
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="77">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -231,6 +231,21 @@
   </si>
   <si>
     <t xml:space="preserve">Lon: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GpsData</t>
   </si>
 </sst>
 </file>
@@ -1914,6 +1929,40 @@
         <v>51</v>
       </c>
     </row>
+    <row r="17">
+      <c r="B17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Divided screens to Debug and Application
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="95">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -246,6 +246,60 @@
   </si>
   <si>
     <t xml:space="preserve">GpsData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01.01.2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Read: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Write: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
   </si>
 </sst>
 </file>
@@ -1727,75 +1781,75 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E7" t="s">
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
         <v>41</v>
@@ -1807,12 +1861,12 @@
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C10" t="s">
         <v>41</v>
@@ -1824,12 +1878,12 @@
         <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
         <v>41</v>
@@ -1841,12 +1895,12 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
         <v>41</v>
@@ -1863,7 +1917,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C13" t="s">
         <v>41</v>
@@ -1875,12 +1929,12 @@
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>41</v>
@@ -1897,7 +1951,7 @@
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C15" t="s">
         <v>41</v>
@@ -1909,12 +1963,12 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C16" t="s">
         <v>41</v>
@@ -1931,36 +1985,206 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E17" t="s">
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="B20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" t="s">
+        <v>43</v>
+      </c>
+      <c r="E20" t="s">
+        <v>44</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>44</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>44</v>
+      </c>
+      <c r="F23" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" t="s">
+        <v>43</v>
+      </c>
+      <c r="E24" t="s">
+        <v>44</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="B25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="B26" t="s">
+        <v>86</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="B27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" t="s">
         <v>38</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D27" t="s">
         <v>73</v>
       </c>
-      <c r="E18" t="s">
-        <v>44</v>
-      </c>
-      <c r="F18" t="s">
-        <v>76</v>
+      <c r="E27" t="s">
+        <v>44</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new debug screens, used custom containers
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="155">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -300,6 +300,186 @@
   </si>
   <si>
     <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug Gps Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Next</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug Draw</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug SD card</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNINITIALIZED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total space: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Free space: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Input files: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output files: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId79</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1961,7 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>38</v>
@@ -1793,12 +1973,12 @@
         <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
         <v>38</v>
@@ -1810,12 +1990,12 @@
         <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -1827,12 +2007,12 @@
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
@@ -1844,15 +2024,15 @@
         <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
         <v>43</v>
@@ -1861,15 +2041,15 @@
         <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>50</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
         <v>43</v>
@@ -1878,15 +2058,15 @@
         <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>55</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -1895,15 +2075,15 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>57</v>
+        <v>98</v>
       </c>
       <c r="C12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
         <v>43</v>
@@ -1912,15 +2092,15 @@
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>43</v>
@@ -1929,15 +2109,15 @@
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>43</v>
@@ -1946,15 +2126,15 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>43</v>
@@ -1963,15 +2143,15 @@
         <v>44</v>
       </c>
       <c r="F15" t="s">
-        <v>62</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D16" t="s">
         <v>43</v>
@@ -1980,15 +2160,15 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>64</v>
+        <v>103</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -1997,12 +2177,12 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="C18" t="s">
         <v>41</v>
@@ -2014,12 +2194,12 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>67</v>
+        <v>105</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -2031,12 +2211,12 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>69</v>
+        <v>106</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -2048,12 +2228,12 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
@@ -2065,12 +2245,12 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -2082,12 +2262,12 @@
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -2099,12 +2279,12 @@
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -2116,12 +2296,12 @@
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>84</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -2133,12 +2313,12 @@
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -2150,41 +2330,449 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="C27" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E27" t="s">
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" t="s">
+        <v>43</v>
+      </c>
+      <c r="E28" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="B29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" t="s">
+        <v>43</v>
+      </c>
+      <c r="E29" t="s">
+        <v>44</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="B30" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>43</v>
+      </c>
+      <c r="E30" t="s">
+        <v>44</v>
+      </c>
+      <c r="F30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="B31" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>43</v>
+      </c>
+      <c r="E31" t="s">
+        <v>44</v>
+      </c>
+      <c r="F31" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="B32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>43</v>
+      </c>
+      <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>43</v>
+      </c>
+      <c r="E34" t="s">
+        <v>44</v>
+      </c>
+      <c r="F34" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="B35" t="s">
+        <v>121</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="B36" t="s">
+        <v>122</v>
+      </c>
+      <c r="C36" t="s">
         <v>38</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D36" t="s">
         <v>73</v>
       </c>
-      <c r="E28" t="s">
-        <v>44</v>
-      </c>
-      <c r="F28" t="s">
-        <v>94</v>
+      <c r="E36" t="s">
+        <v>44</v>
+      </c>
+      <c r="F36" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D37" t="s">
+        <v>73</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="B38" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" t="s">
+        <v>73</v>
+      </c>
+      <c r="E39" t="s">
+        <v>44</v>
+      </c>
+      <c r="F39" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="B40" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D40" t="s">
+        <v>73</v>
+      </c>
+      <c r="E40" t="s">
+        <v>44</v>
+      </c>
+      <c r="F40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="B41" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" t="s">
+        <v>38</v>
+      </c>
+      <c r="D41" t="s">
+        <v>73</v>
+      </c>
+      <c r="E41" t="s">
+        <v>44</v>
+      </c>
+      <c r="F41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="B42" t="s">
+        <v>124</v>
+      </c>
+      <c r="C42" t="s">
+        <v>41</v>
+      </c>
+      <c r="D42" t="s">
+        <v>73</v>
+      </c>
+      <c r="E42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" t="s">
+        <v>43</v>
+      </c>
+      <c r="E43" t="s">
+        <v>44</v>
+      </c>
+      <c r="F43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" t="s">
+        <v>43</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" t="s">
+        <v>43</v>
+      </c>
+      <c r="E45" t="s">
+        <v>44</v>
+      </c>
+      <c r="F45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" t="s">
+        <v>43</v>
+      </c>
+      <c r="E46" t="s">
+        <v>44</v>
+      </c>
+      <c r="F46" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" t="s">
+        <v>146</v>
+      </c>
+      <c r="C47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" t="s">
+        <v>43</v>
+      </c>
+      <c r="E47" t="s">
+        <v>44</v>
+      </c>
+      <c r="F47" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="B48" t="s">
+        <v>148</v>
+      </c>
+      <c r="C48" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" t="s">
+        <v>43</v>
+      </c>
+      <c r="E48" t="s">
+        <v>44</v>
+      </c>
+      <c r="F48" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="B50" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" t="s">
+        <v>43</v>
+      </c>
+      <c r="E50" t="s">
+        <v>44</v>
+      </c>
+      <c r="F50" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" t="s">
+        <v>152</v>
+      </c>
+      <c r="C51" t="s">
+        <v>41</v>
+      </c>
+      <c r="D51" t="s">
+        <v>43</v>
+      </c>
+      <c r="E51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" t="s">
+        <v>154</v>
+      </c>
+      <c r="C52" t="s">
+        <v>41</v>
+      </c>
+      <c r="D52" t="s">
+        <v>43</v>
+      </c>
+      <c r="E52" t="s">
+        <v>44</v>
+      </c>
+      <c r="F52" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added activity application screen and basic logic
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3304" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5191" uniqueCount="186">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -480,6 +480,99 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId87</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NONE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocity: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId89</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0 km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId90</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId91</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance: &lt;value&gt; km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocity: &lt;value&gt; km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AvgVelocity: &lt;value&gt; km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Settings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId97</t>
   </si>
 </sst>
 </file>
@@ -1995,7 +2088,7 @@
     </row>
     <row r="7">
       <c r="B7" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -2007,18 +2100,18 @@
         <v>44</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C8" t="s">
         <v>38</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>44</v>
@@ -2029,7 +2122,7 @@
     </row>
     <row r="9">
       <c r="B9" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -2046,7 +2139,7 @@
     </row>
     <row r="10">
       <c r="B10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
@@ -2063,7 +2156,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2080,7 +2173,7 @@
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -2097,7 +2190,7 @@
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C13" t="s">
         <v>38</v>
@@ -2114,7 +2207,7 @@
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -2131,7 +2224,7 @@
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -2148,7 +2241,7 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -2165,10 +2258,10 @@
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
         <v>43</v>
@@ -2177,12 +2270,12 @@
         <v>44</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C18" t="s">
         <v>41</v>
@@ -2194,12 +2287,12 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -2211,12 +2304,12 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
         <v>41</v>
@@ -2228,12 +2321,12 @@
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C21" t="s">
         <v>41</v>
@@ -2245,12 +2338,12 @@
         <v>44</v>
       </c>
       <c r="F21" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -2262,12 +2355,12 @@
         <v>44</v>
       </c>
       <c r="F22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -2279,12 +2372,12 @@
         <v>44</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -2296,12 +2389,12 @@
         <v>44</v>
       </c>
       <c r="F24" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -2313,12 +2406,12 @@
         <v>44</v>
       </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -2330,12 +2423,12 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -2347,12 +2440,12 @@
         <v>44</v>
       </c>
       <c r="F27" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
@@ -2364,12 +2457,12 @@
         <v>44</v>
       </c>
       <c r="F28" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
@@ -2381,12 +2474,12 @@
         <v>44</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
@@ -2398,12 +2491,12 @@
         <v>44</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -2415,12 +2508,12 @@
         <v>44</v>
       </c>
       <c r="F31" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -2432,12 +2525,12 @@
         <v>44</v>
       </c>
       <c r="F32" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
@@ -2449,12 +2542,12 @@
         <v>44</v>
       </c>
       <c r="F33" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
@@ -2466,32 +2559,32 @@
         <v>44</v>
       </c>
       <c r="F34" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E35" t="s">
         <v>44</v>
       </c>
       <c r="F35" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D36" t="s">
         <v>73</v>
@@ -2500,15 +2593,15 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C37" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
         <v>73</v>
@@ -2517,15 +2610,15 @@
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
         <v>73</v>
@@ -2534,15 +2627,15 @@
         <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C39" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D39" t="s">
         <v>73</v>
@@ -2551,12 +2644,12 @@
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
@@ -2573,41 +2666,41 @@
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D41" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E41" t="s">
         <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>124</v>
+        <v>140</v>
       </c>
       <c r="C42" t="s">
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E42" t="s">
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
         <v>41</v>
@@ -2619,12 +2712,12 @@
         <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C44" t="s">
         <v>41</v>
@@ -2636,12 +2729,12 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C45" t="s">
         <v>41</v>
@@ -2653,12 +2746,12 @@
         <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="C46" t="s">
         <v>41</v>
@@ -2675,7 +2768,7 @@
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C47" t="s">
         <v>41</v>
@@ -2687,12 +2780,12 @@
         <v>44</v>
       </c>
       <c r="F47" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="C48" t="s">
         <v>41</v>
@@ -2709,7 +2802,7 @@
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="C49" t="s">
         <v>41</v>
@@ -2721,12 +2814,12 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C50" t="s">
         <v>41</v>
@@ -2743,7 +2836,7 @@
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="C51" t="s">
         <v>41</v>
@@ -2755,12 +2848,12 @@
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>153</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C52" t="s">
         <v>41</v>
@@ -2772,9 +2865,214 @@
         <v>44</v>
       </c>
       <c r="F52" t="s">
-        <v>145</v>
-      </c>
-    </row>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" t="s">
+        <v>43</v>
+      </c>
+      <c r="E53" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" t="s">
+        <v>163</v>
+      </c>
+      <c r="C54" t="s">
+        <v>41</v>
+      </c>
+      <c r="D54" t="s">
+        <v>43</v>
+      </c>
+      <c r="E54" t="s">
+        <v>44</v>
+      </c>
+      <c r="F54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="B55" t="s">
+        <v>165</v>
+      </c>
+      <c r="C55" t="s">
+        <v>41</v>
+      </c>
+      <c r="D55" t="s">
+        <v>43</v>
+      </c>
+      <c r="E55" t="s">
+        <v>44</v>
+      </c>
+      <c r="F55" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" t="s">
+        <v>167</v>
+      </c>
+      <c r="C56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" t="s">
+        <v>43</v>
+      </c>
+      <c r="E56" t="s">
+        <v>44</v>
+      </c>
+      <c r="F56" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" t="s">
+        <v>169</v>
+      </c>
+      <c r="C57" t="s">
+        <v>41</v>
+      </c>
+      <c r="D57" t="s">
+        <v>43</v>
+      </c>
+      <c r="E57" t="s">
+        <v>44</v>
+      </c>
+      <c r="F57" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" t="s">
+        <v>171</v>
+      </c>
+      <c r="C58" t="s">
+        <v>41</v>
+      </c>
+      <c r="D58" t="s">
+        <v>43</v>
+      </c>
+      <c r="E58" t="s">
+        <v>44</v>
+      </c>
+      <c r="F58" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" t="s">
+        <v>176</v>
+      </c>
+      <c r="C59" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" t="s">
+        <v>43</v>
+      </c>
+      <c r="E59" t="s">
+        <v>44</v>
+      </c>
+      <c r="F59" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" t="s">
+        <v>178</v>
+      </c>
+      <c r="C60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" t="s">
+        <v>43</v>
+      </c>
+      <c r="E60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" t="s">
+        <v>179</v>
+      </c>
+      <c r="C61" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" t="s">
+        <v>73</v>
+      </c>
+      <c r="E61" t="s">
+        <v>44</v>
+      </c>
+      <c r="F61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="B62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D62" t="s">
+        <v>73</v>
+      </c>
+      <c r="E62" t="s">
+        <v>44</v>
+      </c>
+      <c r="F62" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>183</v>
+      </c>
+      <c r="C63" t="s">
+        <v>38</v>
+      </c>
+      <c r="D63" t="s">
+        <v>73</v>
+      </c>
+      <c r="E63" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>185</v>
+      </c>
+      <c r="C64" t="s">
+        <v>38</v>
+      </c>
+      <c r="D64" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" t="s">
+        <v>44</v>
+      </c>
+      <c r="F64" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="65"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Saving track info to gpx file, added app timer
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5191" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5584" uniqueCount="189">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -573,6 +573,15 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId97</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NO FIX</t>
   </si>
 </sst>
 </file>
@@ -3072,7 +3081,40 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65"/>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" t="s">
+        <v>41</v>
+      </c>
+      <c r="D65" t="s">
+        <v>43</v>
+      </c>
+      <c r="E65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>187</v>
+      </c>
+      <c r="C66" t="s">
+        <v>41</v>
+      </c>
+      <c r="D66" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" t="s">
+        <v>188</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added app timer, saving to file when fix is ok
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5584" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="190">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -582,6 +582,9 @@
   </si>
   <si>
     <t xml:space="preserve">NO FIX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:00:00.0</t>
   </si>
 </sst>
 </file>
@@ -2879,7 +2882,7 @@
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="C53" t="s">
         <v>41</v>
@@ -2891,12 +2894,12 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>162</v>
+        <v>174</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C54" t="s">
         <v>41</v>
@@ -2908,12 +2911,12 @@
         <v>44</v>
       </c>
       <c r="F54" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C55" t="s">
         <v>41</v>
@@ -2925,12 +2928,12 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="C56" t="s">
         <v>41</v>
@@ -2942,12 +2945,12 @@
         <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="C57" t="s">
         <v>41</v>
@@ -2959,12 +2962,12 @@
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C58" t="s">
         <v>41</v>
@@ -2976,46 +2979,46 @@
         <v>44</v>
       </c>
       <c r="F58" t="s">
-        <v>53</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="C59" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D59" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E59" t="s">
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="C60" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D60" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E60" t="s">
         <v>44</v>
       </c>
       <c r="F60" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C61" t="s">
         <v>38</v>
@@ -3027,12 +3030,12 @@
         <v>44</v>
       </c>
       <c r="F61" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C62" t="s">
         <v>38</v>
@@ -3047,74 +3050,10 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63">
-      <c r="B63" t="s">
-        <v>183</v>
-      </c>
-      <c r="C63" t="s">
-        <v>38</v>
-      </c>
-      <c r="D63" t="s">
-        <v>73</v>
-      </c>
-      <c r="E63" t="s">
-        <v>44</v>
-      </c>
-      <c r="F63" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="B64" t="s">
-        <v>185</v>
-      </c>
-      <c r="C64" t="s">
-        <v>38</v>
-      </c>
-      <c r="D64" t="s">
-        <v>73</v>
-      </c>
-      <c r="E64" t="s">
-        <v>44</v>
-      </c>
-      <c r="F64" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="B65" t="s">
-        <v>186</v>
-      </c>
-      <c r="C65" t="s">
-        <v>41</v>
-      </c>
-      <c r="D65" t="s">
-        <v>43</v>
-      </c>
-      <c r="E65" t="s">
-        <v>44</v>
-      </c>
-      <c r="F65" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="B66" t="s">
-        <v>187</v>
-      </c>
-      <c r="C66" t="s">
-        <v>41</v>
-      </c>
-      <c r="D66" t="s">
-        <v>43</v>
-      </c>
-      <c r="E66" t="s">
-        <v>44</v>
-      </c>
-      <c r="F66" t="s">
-        <v>188</v>
-      </c>
-    </row>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added activity runtime statistics
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6322" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7429" uniqueCount="195">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -585,6 +585,21 @@
   </si>
   <si>
     <t xml:space="preserve">00:00:00.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed: &lt;value&gt; km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AvgSpeed: &lt;value&gt; km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance: &lt;value&gt; m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed: &lt;value&gt; m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AvgSpeed: &lt;value&gt; m/s</t>
   </si>
 </sst>
 </file>
@@ -2894,7 +2909,7 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>174</v>
+        <v>190</v>
       </c>
     </row>
     <row r="54">
@@ -2962,7 +2977,7 @@
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
     </row>
     <row r="58">

</xml_diff>

<commit_message>
Changed activity user screen
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7429" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9401" uniqueCount="234">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -600,6 +600,125 @@
   </si>
   <si>
     <t xml:space="preserve">AvgSpeed: &lt;value&gt; m/s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narrow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARIALN.TTF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt; km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId103</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId104</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId106</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId107</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId108</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avg speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId110</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Max speed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId112</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId113</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId114</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId115</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId117</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId119</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId120</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId121</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
   </si>
 </sst>
 </file>
@@ -1932,6 +2051,27 @@
       <c r="P6" s="10"/>
     </row>
     <row r="7" spans="2:16">
+      <c r="B7" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" t="s">
+        <v>196</v>
+      </c>
+      <c r="D7">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J7"/>
       <c r="L7" s="7" t="s">
         <v>7</v>
       </c>
@@ -3062,13 +3202,383 @@
         <v>44</v>
       </c>
       <c r="F62" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="63"/>
-    <row r="64"/>
-    <row r="65"/>
-    <row r="66"/>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="B63" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D63" t="s">
+        <v>225</v>
+      </c>
+      <c r="E63" t="s">
+        <v>44</v>
+      </c>
+      <c r="F63" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="B64" t="s">
+        <v>200</v>
+      </c>
+      <c r="C64" t="s">
+        <v>195</v>
+      </c>
+      <c r="D64" t="s">
+        <v>43</v>
+      </c>
+      <c r="E64" t="s">
+        <v>44</v>
+      </c>
+      <c r="F64" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="B65" t="s">
+        <v>201</v>
+      </c>
+      <c r="C65" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" t="s">
+        <v>225</v>
+      </c>
+      <c r="E65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" t="s">
+        <v>203</v>
+      </c>
+      <c r="C66" t="s">
+        <v>195</v>
+      </c>
+      <c r="D66" t="s">
+        <v>43</v>
+      </c>
+      <c r="E66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="B67" t="s">
+        <v>204</v>
+      </c>
+      <c r="C67" t="s">
+        <v>195</v>
+      </c>
+      <c r="D67" t="s">
+        <v>73</v>
+      </c>
+      <c r="E67" t="s">
+        <v>44</v>
+      </c>
+      <c r="F67" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="B68" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" t="s">
+        <v>195</v>
+      </c>
+      <c r="D68" t="s">
+        <v>43</v>
+      </c>
+      <c r="E68" t="s">
+        <v>44</v>
+      </c>
+      <c r="F68" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="B69" t="s">
+        <v>207</v>
+      </c>
+      <c r="C69" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" t="s">
+        <v>73</v>
+      </c>
+      <c r="E69" t="s">
+        <v>44</v>
+      </c>
+      <c r="F69" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="B70" t="s">
+        <v>209</v>
+      </c>
+      <c r="C70" t="s">
+        <v>41</v>
+      </c>
+      <c r="D70" t="s">
+        <v>73</v>
+      </c>
+      <c r="E70" t="s">
+        <v>44</v>
+      </c>
+      <c r="F70" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="B71" t="s">
+        <v>211</v>
+      </c>
+      <c r="C71" t="s">
+        <v>41</v>
+      </c>
+      <c r="D71" t="s">
+        <v>73</v>
+      </c>
+      <c r="E71" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="B72" t="s">
+        <v>213</v>
+      </c>
+      <c r="C72" t="s">
+        <v>41</v>
+      </c>
+      <c r="D72" t="s">
+        <v>73</v>
+      </c>
+      <c r="E72" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="B73" t="s">
+        <v>215</v>
+      </c>
+      <c r="C73" t="s">
+        <v>41</v>
+      </c>
+      <c r="D73" t="s">
+        <v>73</v>
+      </c>
+      <c r="E73" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="B74" t="s">
+        <v>217</v>
+      </c>
+      <c r="C74" t="s">
+        <v>195</v>
+      </c>
+      <c r="D74" t="s">
+        <v>225</v>
+      </c>
+      <c r="E74" t="s">
+        <v>44</v>
+      </c>
+      <c r="F74" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>195</v>
+      </c>
+      <c r="D75" t="s">
+        <v>43</v>
+      </c>
+      <c r="E75" t="s">
+        <v>44</v>
+      </c>
+      <c r="F75" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="B76" t="s">
+        <v>219</v>
+      </c>
+      <c r="C76" t="s">
+        <v>41</v>
+      </c>
+      <c r="D76" t="s">
+        <v>73</v>
+      </c>
+      <c r="E76" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="B77" t="s">
+        <v>221</v>
+      </c>
+      <c r="C77" t="s">
+        <v>195</v>
+      </c>
+      <c r="D77" t="s">
+        <v>73</v>
+      </c>
+      <c r="E77" t="s">
+        <v>44</v>
+      </c>
+      <c r="F77" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="B78" t="s">
+        <v>222</v>
+      </c>
+      <c r="C78" t="s">
+        <v>195</v>
+      </c>
+      <c r="D78" t="s">
+        <v>43</v>
+      </c>
+      <c r="E78" t="s">
+        <v>44</v>
+      </c>
+      <c r="F78" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="B79" t="s">
+        <v>186</v>
+      </c>
+      <c r="C79" t="s">
+        <v>195</v>
+      </c>
+      <c r="D79" t="s">
+        <v>225</v>
+      </c>
+      <c r="E79" t="s">
+        <v>44</v>
+      </c>
+      <c r="F79" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="B80" t="s">
+        <v>226</v>
+      </c>
+      <c r="C80" t="s">
+        <v>41</v>
+      </c>
+      <c r="D80" t="s">
+        <v>43</v>
+      </c>
+      <c r="E80" t="s">
+        <v>44</v>
+      </c>
+      <c r="F80" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="B81" t="s">
+        <v>228</v>
+      </c>
+      <c r="C81" t="s">
+        <v>41</v>
+      </c>
+      <c r="D81" t="s">
+        <v>43</v>
+      </c>
+      <c r="E81" t="s">
+        <v>44</v>
+      </c>
+      <c r="F81" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="B82" t="s">
+        <v>229</v>
+      </c>
+      <c r="C82" t="s">
+        <v>195</v>
+      </c>
+      <c r="D82" t="s">
+        <v>43</v>
+      </c>
+      <c r="E82" t="s">
+        <v>44</v>
+      </c>
+      <c r="F82" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="B83" t="s">
+        <v>230</v>
+      </c>
+      <c r="C83" t="s">
+        <v>41</v>
+      </c>
+      <c r="D83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" t="s">
+        <v>44</v>
+      </c>
+      <c r="F83" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="B84" t="s">
+        <v>231</v>
+      </c>
+      <c r="C84" t="s">
+        <v>41</v>
+      </c>
+      <c r="D84" t="s">
+        <v>43</v>
+      </c>
+      <c r="E84" t="s">
+        <v>44</v>
+      </c>
+      <c r="F84" t="s">
+        <v>232</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added altitude screen, increased stack and head
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9401" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16016" uniqueCount="321">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -715,6 +715,276 @@
   </si>
   <si>
     <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId122</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slope max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId126</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId127</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId129</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alti max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId133</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alti down</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId136</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alti up</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId137</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId138</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId142</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId143</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altitude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId146</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId147</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId149</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId151</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId153</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId154</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId155</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId157</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId158</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId159</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId160</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId161</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId162</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId163</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId164</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId165</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId166</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId167</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId168</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId169</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId170</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId171</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId172</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId173</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId174</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId177</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId178</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId179</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId180</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId181</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId184</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId185</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId188</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId189</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId190</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId191</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId193</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId194</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId195</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId197</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km
+ h</t>
   </si>
   <si>
     <t xml:space="preserve">km
@@ -2748,10 +3018,10 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
         <v>73</v>
@@ -2760,12 +3030,12 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C37" t="s">
         <v>38</v>
@@ -2777,63 +3047,63 @@
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="C38" t="s">
         <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E38" t="s">
         <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C39" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E39" t="s">
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>124</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
@@ -2845,12 +3115,12 @@
         <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>140</v>
+        <v>146</v>
       </c>
       <c r="C42" t="s">
         <v>41</v>
@@ -2862,12 +3132,12 @@
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>41</v>
@@ -2879,12 +3149,12 @@
         <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C44" t="s">
         <v>41</v>
@@ -2896,12 +3166,12 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C45" t="s">
         <v>41</v>
@@ -2913,12 +3183,12 @@
         <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C46" t="s">
         <v>41</v>
@@ -2930,12 +3200,12 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C47" t="s">
         <v>41</v>
@@ -2947,12 +3217,12 @@
         <v>44</v>
       </c>
       <c r="F47" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>151</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
         <v>41</v>
@@ -2964,12 +3234,12 @@
         <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="C49" t="s">
         <v>41</v>
@@ -2981,12 +3251,12 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="C50" t="s">
         <v>41</v>
@@ -2998,12 +3268,12 @@
         <v>44</v>
       </c>
       <c r="F50" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
         <v>41</v>
@@ -3015,12 +3285,12 @@
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>159</v>
+        <v>169</v>
       </c>
       <c r="C52" t="s">
         <v>41</v>
@@ -3032,12 +3302,12 @@
         <v>44</v>
       </c>
       <c r="F52" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>165</v>
+        <v>171</v>
       </c>
       <c r="C53" t="s">
         <v>41</v>
@@ -3049,12 +3319,12 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="C54" t="s">
         <v>41</v>
@@ -3066,12 +3336,12 @@
         <v>44</v>
       </c>
       <c r="F54" t="s">
-        <v>175</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C55" t="s">
         <v>41</v>
@@ -3083,63 +3353,63 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E56" t="s">
         <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C57" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D57" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E57" t="s">
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C58" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D58" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E58" t="s">
         <v>44</v>
       </c>
       <c r="F58" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="C59" t="s">
         <v>38</v>
@@ -3151,134 +3421,134 @@
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="C60" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D60" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E60" t="s">
         <v>44</v>
       </c>
       <c r="F60" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="C61" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E61" t="s">
         <v>44</v>
       </c>
       <c r="F61" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>185</v>
+        <v>201</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E62" t="s">
         <v>44</v>
       </c>
       <c r="F62" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C63" t="s">
         <v>195</v>
       </c>
       <c r="D63" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E63" t="s">
         <v>44</v>
       </c>
       <c r="F63" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C64" t="s">
         <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E64" t="s">
         <v>44</v>
       </c>
       <c r="F64" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="C65" t="s">
         <v>195</v>
       </c>
       <c r="D65" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E65" t="s">
         <v>44</v>
       </c>
       <c r="F65" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C66" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D66" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E66" t="s">
         <v>44</v>
       </c>
       <c r="F66" t="s">
-        <v>173</v>
+        <v>208</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D67" t="s">
         <v>73</v>
@@ -3287,29 +3557,29 @@
         <v>44</v>
       </c>
       <c r="F67" t="s">
-        <v>205</v>
+        <v>210</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="C68" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E68" t="s">
         <v>44</v>
       </c>
       <c r="F68" t="s">
-        <v>189</v>
+        <v>212</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="C69" t="s">
         <v>41</v>
@@ -3321,12 +3591,12 @@
         <v>44</v>
       </c>
       <c r="F69" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>209</v>
+        <v>215</v>
       </c>
       <c r="C70" t="s">
         <v>41</v>
@@ -3338,46 +3608,46 @@
         <v>44</v>
       </c>
       <c r="F70" t="s">
-        <v>210</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="C71" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D71" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E71" t="s">
         <v>44</v>
       </c>
       <c r="F71" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="C72" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D72" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E72" t="s">
         <v>44</v>
       </c>
       <c r="F72" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="C73" t="s">
         <v>41</v>
@@ -3389,18 +3659,18 @@
         <v>44</v>
       </c>
       <c r="F73" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="C74" t="s">
         <v>195</v>
       </c>
       <c r="D74" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E74" t="s">
         <v>44</v>
@@ -3411,7 +3681,7 @@
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C75" t="s">
         <v>195</v>
@@ -3423,49 +3693,49 @@
         <v>44</v>
       </c>
       <c r="F75" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>219</v>
+        <v>186</v>
       </c>
       <c r="C76" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E76" t="s">
         <v>44</v>
       </c>
       <c r="F76" t="s">
-        <v>220</v>
+        <v>205</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>221</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D77" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E77" t="s">
         <v>44</v>
       </c>
       <c r="F77" t="s">
-        <v>205</v>
+        <v>320</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D78" t="s">
         <v>43</v>
@@ -3474,29 +3744,29 @@
         <v>44</v>
       </c>
       <c r="F78" t="s">
-        <v>223</v>
+        <v>320</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>186</v>
+        <v>229</v>
       </c>
       <c r="C79" t="s">
         <v>195</v>
       </c>
       <c r="D79" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E79" t="s">
         <v>44</v>
       </c>
       <c r="F79" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="C80" t="s">
         <v>41</v>
@@ -3508,12 +3778,12 @@
         <v>44</v>
       </c>
       <c r="F80" t="s">
-        <v>233</v>
+        <v>320</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C81" t="s">
         <v>41</v>
@@ -3525,32 +3795,32 @@
         <v>44</v>
       </c>
       <c r="F81" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="C82" t="s">
         <v>195</v>
       </c>
       <c r="D82" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E82" t="s">
         <v>44</v>
       </c>
       <c r="F82" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="C83" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
         <v>43</v>
@@ -3559,24 +3829,1163 @@
         <v>44</v>
       </c>
       <c r="F83" t="s">
-        <v>233</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="C84" t="s">
         <v>41</v>
       </c>
       <c r="D84" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E84" t="s">
         <v>44</v>
       </c>
       <c r="F84" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="B85" t="s">
+        <v>239</v>
+      </c>
+      <c r="C85" t="s">
+        <v>195</v>
+      </c>
+      <c r="D85" t="s">
+        <v>225</v>
+      </c>
+      <c r="E85" t="s">
+        <v>44</v>
+      </c>
+      <c r="F85" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="B86" t="s">
+        <v>240</v>
+      </c>
+      <c r="C86" t="s">
+        <v>195</v>
+      </c>
+      <c r="D86" t="s">
+        <v>43</v>
+      </c>
+      <c r="E86" t="s">
+        <v>44</v>
+      </c>
+      <c r="F86" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="B87" t="s">
+        <v>241</v>
+      </c>
+      <c r="C87" t="s">
+        <v>41</v>
+      </c>
+      <c r="D87" t="s">
+        <v>73</v>
+      </c>
+      <c r="E87" t="s">
+        <v>44</v>
+      </c>
+      <c r="F87" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="B88" t="s">
+        <v>243</v>
+      </c>
+      <c r="C88" t="s">
+        <v>41</v>
+      </c>
+      <c r="D88" t="s">
+        <v>73</v>
+      </c>
+      <c r="E88" t="s">
+        <v>44</v>
+      </c>
+      <c r="F88" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="B89" t="s">
+        <v>245</v>
+      </c>
+      <c r="C89" t="s">
+        <v>41</v>
+      </c>
+      <c r="D89" t="s">
+        <v>73</v>
+      </c>
+      <c r="E89" t="s">
+        <v>44</v>
+      </c>
+      <c r="F89" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="B90" t="s">
+        <v>247</v>
+      </c>
+      <c r="C90" t="s">
+        <v>195</v>
+      </c>
+      <c r="D90" t="s">
+        <v>225</v>
+      </c>
+      <c r="E90" t="s">
+        <v>44</v>
+      </c>
+      <c r="F90" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="B91" t="s">
+        <v>248</v>
+      </c>
+      <c r="C91" t="s">
+        <v>195</v>
+      </c>
+      <c r="D91" t="s">
+        <v>43</v>
+      </c>
+      <c r="E91" t="s">
+        <v>44</v>
+      </c>
+      <c r="F91" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="B92" t="s">
+        <v>249</v>
+      </c>
+      <c r="C92" t="s">
+        <v>41</v>
+      </c>
+      <c r="D92" t="s">
+        <v>43</v>
+      </c>
+      <c r="E92" t="s">
+        <v>44</v>
+      </c>
+      <c r="F92" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="B93" t="s">
+        <v>251</v>
+      </c>
+      <c r="C93" t="s">
+        <v>41</v>
+      </c>
+      <c r="D93" t="s">
+        <v>73</v>
+      </c>
+      <c r="E93" t="s">
+        <v>44</v>
+      </c>
+      <c r="F93" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="B94" t="s">
+        <v>253</v>
+      </c>
+      <c r="C94" t="s">
+        <v>195</v>
+      </c>
+      <c r="D94" t="s">
+        <v>225</v>
+      </c>
+      <c r="E94" t="s">
+        <v>44</v>
+      </c>
+      <c r="F94" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="B95" t="s">
+        <v>254</v>
+      </c>
+      <c r="C95" t="s">
+        <v>195</v>
+      </c>
+      <c r="D95" t="s">
+        <v>43</v>
+      </c>
+      <c r="E95" t="s">
+        <v>44</v>
+      </c>
+      <c r="F95" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="B96" t="s">
+        <v>255</v>
+      </c>
+      <c r="C96" t="s">
+        <v>41</v>
+      </c>
+      <c r="D96" t="s">
+        <v>73</v>
+      </c>
+      <c r="E96" t="s">
+        <v>44</v>
+      </c>
+      <c r="F96" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="B97" t="s">
+        <v>257</v>
+      </c>
+      <c r="C97" t="s">
+        <v>41</v>
+      </c>
+      <c r="D97" t="s">
+        <v>43</v>
+      </c>
+      <c r="E97" t="s">
+        <v>44</v>
+      </c>
+      <c r="F97" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="B98" t="s">
+        <v>259</v>
+      </c>
+      <c r="C98" t="s">
+        <v>41</v>
+      </c>
+      <c r="D98" t="s">
+        <v>43</v>
+      </c>
+      <c r="E98" t="s">
+        <v>44</v>
+      </c>
+      <c r="F98" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="B99" t="s">
+        <v>260</v>
+      </c>
+      <c r="C99" t="s">
+        <v>41</v>
+      </c>
+      <c r="D99" t="s">
+        <v>43</v>
+      </c>
+      <c r="E99" t="s">
+        <v>44</v>
+      </c>
+      <c r="F99" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="B100" t="s">
+        <v>261</v>
+      </c>
+      <c r="C100" t="s">
+        <v>195</v>
+      </c>
+      <c r="D100" t="s">
+        <v>225</v>
+      </c>
+      <c r="E100" t="s">
+        <v>44</v>
+      </c>
+      <c r="F100" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="B101" t="s">
+        <v>262</v>
+      </c>
+      <c r="C101" t="s">
+        <v>195</v>
+      </c>
+      <c r="D101" t="s">
+        <v>43</v>
+      </c>
+      <c r="E101" t="s">
+        <v>44</v>
+      </c>
+      <c r="F101" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="B102" t="s">
+        <v>263</v>
+      </c>
+      <c r="C102" t="s">
+        <v>41</v>
+      </c>
+      <c r="D102" t="s">
+        <v>43</v>
+      </c>
+      <c r="E102" t="s">
+        <v>44</v>
+      </c>
+      <c r="F102" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="B103" t="s">
+        <v>264</v>
+      </c>
+      <c r="C103" t="s">
+        <v>195</v>
+      </c>
+      <c r="D103" t="s">
+        <v>225</v>
+      </c>
+      <c r="E103" t="s">
+        <v>44</v>
+      </c>
+      <c r="F103" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="B104" t="s">
+        <v>265</v>
+      </c>
+      <c r="C104" t="s">
+        <v>195</v>
+      </c>
+      <c r="D104" t="s">
+        <v>43</v>
+      </c>
+      <c r="E104" t="s">
+        <v>44</v>
+      </c>
+      <c r="F104" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="B105" t="s">
+        <v>266</v>
+      </c>
+      <c r="C105" t="s">
+        <v>41</v>
+      </c>
+      <c r="D105" t="s">
+        <v>43</v>
+      </c>
+      <c r="E105" t="s">
+        <v>44</v>
+      </c>
+      <c r="F105" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="B106" t="s">
+        <v>273</v>
+      </c>
+      <c r="C106" t="s">
+        <v>195</v>
+      </c>
+      <c r="D106" t="s">
+        <v>225</v>
+      </c>
+      <c r="E106" t="s">
+        <v>44</v>
+      </c>
+      <c r="F106" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="B107" t="s">
+        <v>274</v>
+      </c>
+      <c r="C107" t="s">
+        <v>195</v>
+      </c>
+      <c r="D107" t="s">
+        <v>43</v>
+      </c>
+      <c r="E107" t="s">
+        <v>44</v>
+      </c>
+      <c r="F107" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="B108" t="s">
+        <v>275</v>
+      </c>
+      <c r="C108" t="s">
+        <v>41</v>
+      </c>
+      <c r="D108" t="s">
+        <v>43</v>
+      </c>
+      <c r="E108" t="s">
+        <v>44</v>
+      </c>
+      <c r="F108" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="B109" t="s">
+        <v>276</v>
+      </c>
+      <c r="C109" t="s">
+        <v>41</v>
+      </c>
+      <c r="D109" t="s">
+        <v>73</v>
+      </c>
+      <c r="E109" t="s">
+        <v>44</v>
+      </c>
+      <c r="F109" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="B110" t="s">
+        <v>277</v>
+      </c>
+      <c r="C110" t="s">
+        <v>195</v>
+      </c>
+      <c r="D110" t="s">
+        <v>225</v>
+      </c>
+      <c r="E110" t="s">
+        <v>44</v>
+      </c>
+      <c r="F110" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="B111" t="s">
+        <v>278</v>
+      </c>
+      <c r="C111" t="s">
+        <v>195</v>
+      </c>
+      <c r="D111" t="s">
+        <v>43</v>
+      </c>
+      <c r="E111" t="s">
+        <v>44</v>
+      </c>
+      <c r="F111" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="B112" t="s">
+        <v>279</v>
+      </c>
+      <c r="C112" t="s">
+        <v>41</v>
+      </c>
+      <c r="D112" t="s">
+        <v>43</v>
+      </c>
+      <c r="E112" t="s">
+        <v>44</v>
+      </c>
+      <c r="F112" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="B113" t="s">
+        <v>280</v>
+      </c>
+      <c r="C113" t="s">
+        <v>41</v>
+      </c>
+      <c r="D113" t="s">
+        <v>73</v>
+      </c>
+      <c r="E113" t="s">
+        <v>44</v>
+      </c>
+      <c r="F113" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="B114" t="s">
+        <v>281</v>
+      </c>
+      <c r="C114" t="s">
+        <v>195</v>
+      </c>
+      <c r="D114" t="s">
+        <v>225</v>
+      </c>
+      <c r="E114" t="s">
+        <v>44</v>
+      </c>
+      <c r="F114" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="B115" t="s">
+        <v>282</v>
+      </c>
+      <c r="C115" t="s">
+        <v>195</v>
+      </c>
+      <c r="D115" t="s">
+        <v>43</v>
+      </c>
+      <c r="E115" t="s">
+        <v>44</v>
+      </c>
+      <c r="F115" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="B116" t="s">
+        <v>283</v>
+      </c>
+      <c r="C116" t="s">
+        <v>41</v>
+      </c>
+      <c r="D116" t="s">
+        <v>43</v>
+      </c>
+      <c r="E116" t="s">
+        <v>44</v>
+      </c>
+      <c r="F116" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="B117" t="s">
+        <v>284</v>
+      </c>
+      <c r="C117" t="s">
+        <v>41</v>
+      </c>
+      <c r="D117" t="s">
+        <v>73</v>
+      </c>
+      <c r="E117" t="s">
+        <v>44</v>
+      </c>
+      <c r="F117" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="B118" t="s">
+        <v>285</v>
+      </c>
+      <c r="C118" t="s">
+        <v>195</v>
+      </c>
+      <c r="D118" t="s">
+        <v>225</v>
+      </c>
+      <c r="E118" t="s">
+        <v>44</v>
+      </c>
+      <c r="F118" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="B119" t="s">
+        <v>286</v>
+      </c>
+      <c r="C119" t="s">
+        <v>195</v>
+      </c>
+      <c r="D119" t="s">
+        <v>43</v>
+      </c>
+      <c r="E119" t="s">
+        <v>44</v>
+      </c>
+      <c r="F119" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="B120" t="s">
+        <v>287</v>
+      </c>
+      <c r="C120" t="s">
+        <v>41</v>
+      </c>
+      <c r="D120" t="s">
+        <v>43</v>
+      </c>
+      <c r="E120" t="s">
+        <v>44</v>
+      </c>
+      <c r="F120" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="B121" t="s">
+        <v>288</v>
+      </c>
+      <c r="C121" t="s">
+        <v>41</v>
+      </c>
+      <c r="D121" t="s">
+        <v>73</v>
+      </c>
+      <c r="E121" t="s">
+        <v>44</v>
+      </c>
+      <c r="F121" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="B122" t="s">
+        <v>289</v>
+      </c>
+      <c r="C122" t="s">
+        <v>195</v>
+      </c>
+      <c r="D122" t="s">
+        <v>225</v>
+      </c>
+      <c r="E122" t="s">
+        <v>44</v>
+      </c>
+      <c r="F122" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="B123" t="s">
+        <v>290</v>
+      </c>
+      <c r="C123" t="s">
+        <v>195</v>
+      </c>
+      <c r="D123" t="s">
+        <v>43</v>
+      </c>
+      <c r="E123" t="s">
+        <v>44</v>
+      </c>
+      <c r="F123" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="B124" t="s">
+        <v>291</v>
+      </c>
+      <c r="C124" t="s">
+        <v>41</v>
+      </c>
+      <c r="D124" t="s">
+        <v>43</v>
+      </c>
+      <c r="E124" t="s">
+        <v>44</v>
+      </c>
+      <c r="F124" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="B125" t="s">
+        <v>292</v>
+      </c>
+      <c r="C125" t="s">
+        <v>41</v>
+      </c>
+      <c r="D125" t="s">
+        <v>73</v>
+      </c>
+      <c r="E125" t="s">
+        <v>44</v>
+      </c>
+      <c r="F125" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="B126" t="s">
+        <v>293</v>
+      </c>
+      <c r="C126" t="s">
+        <v>195</v>
+      </c>
+      <c r="D126" t="s">
+        <v>225</v>
+      </c>
+      <c r="E126" t="s">
+        <v>44</v>
+      </c>
+      <c r="F126" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="B127" t="s">
+        <v>294</v>
+      </c>
+      <c r="C127" t="s">
+        <v>195</v>
+      </c>
+      <c r="D127" t="s">
+        <v>43</v>
+      </c>
+      <c r="E127" t="s">
+        <v>44</v>
+      </c>
+      <c r="F127" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="B128" t="s">
+        <v>295</v>
+      </c>
+      <c r="C128" t="s">
+        <v>41</v>
+      </c>
+      <c r="D128" t="s">
+        <v>43</v>
+      </c>
+      <c r="E128" t="s">
+        <v>44</v>
+      </c>
+      <c r="F128" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="B129" t="s">
+        <v>296</v>
+      </c>
+      <c r="C129" t="s">
+        <v>41</v>
+      </c>
+      <c r="D129" t="s">
+        <v>73</v>
+      </c>
+      <c r="E129" t="s">
+        <v>44</v>
+      </c>
+      <c r="F129" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="B130" t="s">
+        <v>297</v>
+      </c>
+      <c r="C130" t="s">
+        <v>195</v>
+      </c>
+      <c r="D130" t="s">
+        <v>225</v>
+      </c>
+      <c r="E130" t="s">
+        <v>44</v>
+      </c>
+      <c r="F130" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="B131" t="s">
+        <v>298</v>
+      </c>
+      <c r="C131" t="s">
+        <v>195</v>
+      </c>
+      <c r="D131" t="s">
+        <v>43</v>
+      </c>
+      <c r="E131" t="s">
+        <v>44</v>
+      </c>
+      <c r="F131" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="B132" t="s">
+        <v>299</v>
+      </c>
+      <c r="C132" t="s">
+        <v>41</v>
+      </c>
+      <c r="D132" t="s">
+        <v>43</v>
+      </c>
+      <c r="E132" t="s">
+        <v>44</v>
+      </c>
+      <c r="F132" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="B133" t="s">
+        <v>300</v>
+      </c>
+      <c r="C133" t="s">
+        <v>41</v>
+      </c>
+      <c r="D133" t="s">
+        <v>73</v>
+      </c>
+      <c r="E133" t="s">
+        <v>44</v>
+      </c>
+      <c r="F133" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="B134" t="s">
+        <v>301</v>
+      </c>
+      <c r="C134" t="s">
+        <v>195</v>
+      </c>
+      <c r="D134" t="s">
+        <v>225</v>
+      </c>
+      <c r="E134" t="s">
+        <v>44</v>
+      </c>
+      <c r="F134" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="B135" t="s">
+        <v>302</v>
+      </c>
+      <c r="C135" t="s">
+        <v>195</v>
+      </c>
+      <c r="D135" t="s">
+        <v>43</v>
+      </c>
+      <c r="E135" t="s">
+        <v>44</v>
+      </c>
+      <c r="F135" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="B136" t="s">
+        <v>303</v>
+      </c>
+      <c r="C136" t="s">
+        <v>41</v>
+      </c>
+      <c r="D136" t="s">
+        <v>43</v>
+      </c>
+      <c r="E136" t="s">
+        <v>44</v>
+      </c>
+      <c r="F136" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="B137" t="s">
+        <v>304</v>
+      </c>
+      <c r="C137" t="s">
+        <v>41</v>
+      </c>
+      <c r="D137" t="s">
+        <v>73</v>
+      </c>
+      <c r="E137" t="s">
+        <v>44</v>
+      </c>
+      <c r="F137" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="B138" t="s">
+        <v>305</v>
+      </c>
+      <c r="C138" t="s">
+        <v>195</v>
+      </c>
+      <c r="D138" t="s">
+        <v>225</v>
+      </c>
+      <c r="E138" t="s">
+        <v>44</v>
+      </c>
+      <c r="F138" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="B139" t="s">
+        <v>306</v>
+      </c>
+      <c r="C139" t="s">
+        <v>195</v>
+      </c>
+      <c r="D139" t="s">
+        <v>43</v>
+      </c>
+      <c r="E139" t="s">
+        <v>44</v>
+      </c>
+      <c r="F139" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="B140" t="s">
+        <v>307</v>
+      </c>
+      <c r="C140" t="s">
+        <v>41</v>
+      </c>
+      <c r="D140" t="s">
+        <v>43</v>
+      </c>
+      <c r="E140" t="s">
+        <v>44</v>
+      </c>
+      <c r="F140" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="B141" t="s">
+        <v>308</v>
+      </c>
+      <c r="C141" t="s">
+        <v>41</v>
+      </c>
+      <c r="D141" t="s">
+        <v>73</v>
+      </c>
+      <c r="E141" t="s">
+        <v>44</v>
+      </c>
+      <c r="F141" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="B142" t="s">
+        <v>309</v>
+      </c>
+      <c r="C142" t="s">
+        <v>195</v>
+      </c>
+      <c r="D142" t="s">
+        <v>73</v>
+      </c>
+      <c r="E142" t="s">
+        <v>44</v>
+      </c>
+      <c r="F142" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="B143" t="s">
+        <v>310</v>
+      </c>
+      <c r="C143" t="s">
+        <v>195</v>
+      </c>
+      <c r="D143" t="s">
+        <v>43</v>
+      </c>
+      <c r="E143" t="s">
+        <v>44</v>
+      </c>
+      <c r="F143" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="B144" t="s">
+        <v>311</v>
+      </c>
+      <c r="C144" t="s">
+        <v>41</v>
+      </c>
+      <c r="D144" t="s">
+        <v>73</v>
+      </c>
+      <c r="E144" t="s">
+        <v>44</v>
+      </c>
+      <c r="F144" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="B145" t="s">
+        <v>312</v>
+      </c>
+      <c r="C145" t="s">
+        <v>195</v>
+      </c>
+      <c r="D145" t="s">
+        <v>225</v>
+      </c>
+      <c r="E145" t="s">
+        <v>44</v>
+      </c>
+      <c r="F145" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="B146" t="s">
+        <v>313</v>
+      </c>
+      <c r="C146" t="s">
+        <v>195</v>
+      </c>
+      <c r="D146" t="s">
+        <v>43</v>
+      </c>
+      <c r="E146" t="s">
+        <v>44</v>
+      </c>
+      <c r="F146" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="B147" t="s">
+        <v>314</v>
+      </c>
+      <c r="C147" t="s">
+        <v>41</v>
+      </c>
+      <c r="D147" t="s">
+        <v>43</v>
+      </c>
+      <c r="E147" t="s">
+        <v>44</v>
+      </c>
+      <c r="F147" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="B148" t="s">
+        <v>315</v>
+      </c>
+      <c r="C148" t="s">
+        <v>41</v>
+      </c>
+      <c r="D148" t="s">
+        <v>73</v>
+      </c>
+      <c r="E148" t="s">
+        <v>44</v>
+      </c>
+      <c r="F148" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="B149" t="s">
+        <v>316</v>
+      </c>
+      <c r="C149" t="s">
+        <v>195</v>
+      </c>
+      <c r="D149" t="s">
+        <v>73</v>
+      </c>
+      <c r="E149" t="s">
+        <v>44</v>
+      </c>
+      <c r="F149" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="B150" t="s">
+        <v>317</v>
+      </c>
+      <c r="C150" t="s">
+        <v>195</v>
+      </c>
+      <c r="D150" t="s">
+        <v>43</v>
+      </c>
+      <c r="E150" t="s">
+        <v>44</v>
+      </c>
+      <c r="F150" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="B151" t="s">
+        <v>318</v>
+      </c>
+      <c r="C151" t="s">
+        <v>41</v>
+      </c>
+      <c r="D151" t="s">
+        <v>73</v>
+      </c>
+      <c r="E151" t="s">
+        <v>44</v>
+      </c>
+      <c r="F151" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added altimeter config and basic readouts
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16016" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18034" uniqueCount="348">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -989,6 +989,87 @@
   <si>
     <t xml:space="preserve">km
  h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId199</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debug EnvSensors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId201</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId203</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId206</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId207</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId208</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId209</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId214</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId215</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId216</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId217</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 hPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId218</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altitude: &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId219</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.00 m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperature: &lt;value&gt; C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure: &lt;value&gt; hPa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Altitude: &lt;value&gt; m</t>
   </si>
 </sst>
 </file>
@@ -3727,7 +3808,7 @@
         <v>44</v>
       </c>
       <c r="F77" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78">
@@ -3744,7 +3825,7 @@
         <v>44</v>
       </c>
       <c r="F78" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79">
@@ -3778,7 +3859,7 @@
         <v>44</v>
       </c>
       <c r="F80" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="81">
@@ -4662,7 +4743,7 @@
         <v>44</v>
       </c>
       <c r="F132" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="133">
@@ -4730,7 +4811,7 @@
         <v>44</v>
       </c>
       <c r="F136" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="137">
@@ -4798,7 +4879,7 @@
         <v>44</v>
       </c>
       <c r="F140" t="s">
-        <v>320</v>
+        <v>227</v>
       </c>
     </row>
     <row r="141">
@@ -4986,6 +5067,295 @@
       </c>
       <c r="F151" t="s">
         <v>208</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="B152" t="s">
+        <v>321</v>
+      </c>
+      <c r="C152" t="s">
+        <v>38</v>
+      </c>
+      <c r="D152" t="s">
+        <v>73</v>
+      </c>
+      <c r="E152" t="s">
+        <v>44</v>
+      </c>
+      <c r="F152" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="B153" t="s">
+        <v>323</v>
+      </c>
+      <c r="C153" t="s">
+        <v>41</v>
+      </c>
+      <c r="D153" t="s">
+        <v>43</v>
+      </c>
+      <c r="E153" t="s">
+        <v>44</v>
+      </c>
+      <c r="F153" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="B154" t="s">
+        <v>324</v>
+      </c>
+      <c r="C154" t="s">
+        <v>41</v>
+      </c>
+      <c r="D154" t="s">
+        <v>43</v>
+      </c>
+      <c r="E154" t="s">
+        <v>44</v>
+      </c>
+      <c r="F154" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="B155" t="s">
+        <v>325</v>
+      </c>
+      <c r="C155" t="s">
+        <v>41</v>
+      </c>
+      <c r="D155" t="s">
+        <v>43</v>
+      </c>
+      <c r="E155" t="s">
+        <v>44</v>
+      </c>
+      <c r="F155" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="B156" t="s">
+        <v>326</v>
+      </c>
+      <c r="C156" t="s">
+        <v>41</v>
+      </c>
+      <c r="D156" t="s">
+        <v>43</v>
+      </c>
+      <c r="E156" t="s">
+        <v>44</v>
+      </c>
+      <c r="F156" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="B157" t="s">
+        <v>327</v>
+      </c>
+      <c r="C157" t="s">
+        <v>41</v>
+      </c>
+      <c r="D157" t="s">
+        <v>43</v>
+      </c>
+      <c r="E157" t="s">
+        <v>44</v>
+      </c>
+      <c r="F157" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="B158" t="s">
+        <v>328</v>
+      </c>
+      <c r="C158" t="s">
+        <v>41</v>
+      </c>
+      <c r="D158" t="s">
+        <v>43</v>
+      </c>
+      <c r="E158" t="s">
+        <v>44</v>
+      </c>
+      <c r="F158" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="B159" t="s">
+        <v>329</v>
+      </c>
+      <c r="C159" t="s">
+        <v>41</v>
+      </c>
+      <c r="D159" t="s">
+        <v>43</v>
+      </c>
+      <c r="E159" t="s">
+        <v>44</v>
+      </c>
+      <c r="F159" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="B160" t="s">
+        <v>330</v>
+      </c>
+      <c r="C160" t="s">
+        <v>41</v>
+      </c>
+      <c r="D160" t="s">
+        <v>43</v>
+      </c>
+      <c r="E160" t="s">
+        <v>44</v>
+      </c>
+      <c r="F160" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="B161" t="s">
+        <v>331</v>
+      </c>
+      <c r="C161" t="s">
+        <v>41</v>
+      </c>
+      <c r="D161" t="s">
+        <v>43</v>
+      </c>
+      <c r="E161" t="s">
+        <v>44</v>
+      </c>
+      <c r="F161" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" t="s">
+        <v>332</v>
+      </c>
+      <c r="C162" t="s">
+        <v>41</v>
+      </c>
+      <c r="D162" t="s">
+        <v>43</v>
+      </c>
+      <c r="E162" t="s">
+        <v>44</v>
+      </c>
+      <c r="F162" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" t="s">
+        <v>333</v>
+      </c>
+      <c r="C163" t="s">
+        <v>41</v>
+      </c>
+      <c r="D163" t="s">
+        <v>43</v>
+      </c>
+      <c r="E163" t="s">
+        <v>44</v>
+      </c>
+      <c r="F163" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="B164" t="s">
+        <v>335</v>
+      </c>
+      <c r="C164" t="s">
+        <v>41</v>
+      </c>
+      <c r="D164" t="s">
+        <v>43</v>
+      </c>
+      <c r="E164" t="s">
+        <v>44</v>
+      </c>
+      <c r="F164" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" t="s">
+        <v>337</v>
+      </c>
+      <c r="C165" t="s">
+        <v>41</v>
+      </c>
+      <c r="D165" t="s">
+        <v>43</v>
+      </c>
+      <c r="E165" t="s">
+        <v>44</v>
+      </c>
+      <c r="F165" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="s">
+        <v>339</v>
+      </c>
+      <c r="C166" t="s">
+        <v>41</v>
+      </c>
+      <c r="D166" t="s">
+        <v>43</v>
+      </c>
+      <c r="E166" t="s">
+        <v>44</v>
+      </c>
+      <c r="F166" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="s">
+        <v>341</v>
+      </c>
+      <c r="C167" t="s">
+        <v>41</v>
+      </c>
+      <c r="D167" t="s">
+        <v>43</v>
+      </c>
+      <c r="E167" t="s">
+        <v>44</v>
+      </c>
+      <c r="F167" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="s">
+        <v>343</v>
+      </c>
+      <c r="C168" t="s">
+        <v>41</v>
+      </c>
+      <c r="D168" t="s">
+        <v>43</v>
+      </c>
+      <c r="E168" t="s">
+        <v>44</v>
+      </c>
+      <c r="F168" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed old container, added map container
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18034" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18995" uniqueCount="348">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -3303,95 +3303,95 @@
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="C48" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D48" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E48" t="s">
         <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>159</v>
+        <v>181</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D49" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E49" t="s">
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>165</v>
+        <v>183</v>
       </c>
       <c r="C50" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D50" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E50" t="s">
         <v>44</v>
       </c>
       <c r="F50" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>167</v>
+        <v>185</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D51" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E51" t="s">
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
       <c r="C52" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D52" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E52" t="s">
         <v>44</v>
       </c>
       <c r="F52" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="C53" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D53" t="s">
         <v>43</v>
@@ -3400,32 +3400,32 @@
         <v>44</v>
       </c>
       <c r="F53" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>176</v>
+        <v>201</v>
       </c>
       <c r="C54" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D54" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E54" t="s">
         <v>44</v>
       </c>
       <c r="F54" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>178</v>
+        <v>203</v>
       </c>
       <c r="C55" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D55" t="s">
         <v>43</v>
@@ -3434,15 +3434,15 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>179</v>
+        <v>204</v>
       </c>
       <c r="C56" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D56" t="s">
         <v>73</v>
@@ -3451,32 +3451,32 @@
         <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>180</v>
+        <v>205</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>181</v>
+        <v>206</v>
       </c>
       <c r="C57" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D57" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E57" t="s">
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>183</v>
+        <v>207</v>
       </c>
       <c r="C58" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D58" t="s">
         <v>73</v>
@@ -3485,15 +3485,15 @@
         <v>44</v>
       </c>
       <c r="F58" t="s">
-        <v>184</v>
+        <v>208</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c r="C59" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D59" t="s">
         <v>73</v>
@@ -3502,117 +3502,117 @@
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>199</v>
+        <v>211</v>
       </c>
       <c r="C60" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D60" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E60" t="s">
         <v>44</v>
       </c>
       <c r="F60" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="C61" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D61" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E61" t="s">
         <v>44</v>
       </c>
       <c r="F61" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="C62" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D62" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E62" t="s">
         <v>44</v>
       </c>
       <c r="F62" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>203</v>
+        <v>217</v>
       </c>
       <c r="C63" t="s">
         <v>195</v>
       </c>
       <c r="D63" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E63" t="s">
         <v>44</v>
       </c>
       <c r="F63" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="C64" t="s">
         <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E64" t="s">
         <v>44</v>
       </c>
       <c r="F64" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>206</v>
+        <v>219</v>
       </c>
       <c r="C65" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D65" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E65" t="s">
         <v>44</v>
       </c>
       <c r="F65" t="s">
-        <v>189</v>
+        <v>220</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="C66" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D66" t="s">
         <v>73</v>
@@ -3621,100 +3621,100 @@
         <v>44</v>
       </c>
       <c r="F66" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="C67" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D67" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E67" t="s">
         <v>44</v>
       </c>
       <c r="F67" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>211</v>
+        <v>186</v>
       </c>
       <c r="C68" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E68" t="s">
         <v>44</v>
       </c>
       <c r="F68" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>213</v>
+        <v>226</v>
       </c>
       <c r="C69" t="s">
         <v>41</v>
       </c>
       <c r="D69" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E69" t="s">
         <v>44</v>
       </c>
       <c r="F69" t="s">
-        <v>214</v>
+        <v>227</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
       <c r="C70" t="s">
         <v>41</v>
       </c>
       <c r="D70" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E70" t="s">
         <v>44</v>
       </c>
       <c r="F70" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="C71" t="s">
         <v>195</v>
       </c>
       <c r="D71" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E71" t="s">
         <v>44</v>
       </c>
       <c r="F71" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="C72" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D72" t="s">
         <v>43</v>
@@ -3723,35 +3723,35 @@
         <v>44</v>
       </c>
       <c r="F72" t="s">
-        <v>173</v>
+        <v>227</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C73" t="s">
         <v>41</v>
       </c>
       <c r="D73" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E73" t="s">
         <v>44</v>
       </c>
       <c r="F73" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>221</v>
+        <v>235</v>
       </c>
       <c r="C74" t="s">
         <v>195</v>
       </c>
       <c r="D74" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E74" t="s">
         <v>44</v>
@@ -3762,7 +3762,7 @@
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>222</v>
+        <v>236</v>
       </c>
       <c r="C75" t="s">
         <v>195</v>
@@ -3774,49 +3774,49 @@
         <v>44</v>
       </c>
       <c r="F75" t="s">
-        <v>223</v>
+        <v>175</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>186</v>
+        <v>237</v>
       </c>
       <c r="C76" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D76" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E76" t="s">
         <v>44</v>
       </c>
       <c r="F76" t="s">
-        <v>205</v>
+        <v>238</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c r="C77" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D77" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E77" t="s">
         <v>44</v>
       </c>
       <c r="F77" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="C78" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D78" t="s">
         <v>43</v>
@@ -3825,63 +3825,63 @@
         <v>44</v>
       </c>
       <c r="F78" t="s">
-        <v>227</v>
+        <v>145</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="C79" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D79" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E79" t="s">
         <v>44</v>
       </c>
       <c r="F79" t="s">
-        <v>173</v>
+        <v>242</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="C80" t="s">
         <v>41</v>
       </c>
       <c r="D80" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E80" t="s">
         <v>44</v>
       </c>
       <c r="F80" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>231</v>
+        <v>245</v>
       </c>
       <c r="C81" t="s">
         <v>41</v>
       </c>
       <c r="D81" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E81" t="s">
         <v>44</v>
       </c>
       <c r="F81" t="s">
-        <v>232</v>
+        <v>246</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C82" t="s">
         <v>195</v>
@@ -3898,7 +3898,7 @@
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="C83" t="s">
         <v>195</v>
@@ -3915,75 +3915,75 @@
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C84" t="s">
         <v>41</v>
       </c>
       <c r="D84" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E84" t="s">
         <v>44</v>
       </c>
       <c r="F84" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="C85" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D85" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E85" t="s">
         <v>44</v>
       </c>
       <c r="F85" t="s">
-        <v>205</v>
+        <v>252</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>240</v>
+        <v>253</v>
       </c>
       <c r="C86" t="s">
         <v>195</v>
       </c>
       <c r="D86" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E86" t="s">
         <v>44</v>
       </c>
       <c r="F86" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>241</v>
+        <v>254</v>
       </c>
       <c r="C87" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D87" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E87" t="s">
         <v>44</v>
       </c>
       <c r="F87" t="s">
-        <v>242</v>
+        <v>145</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="C88" t="s">
         <v>41</v>
@@ -3995,49 +3995,49 @@
         <v>44</v>
       </c>
       <c r="F88" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="C89" t="s">
         <v>41</v>
       </c>
       <c r="D89" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E89" t="s">
         <v>44</v>
       </c>
       <c r="F89" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="C90" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D90" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E90" t="s">
         <v>44</v>
       </c>
       <c r="F90" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="C91" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D91" t="s">
         <v>43</v>
@@ -4046,97 +4046,97 @@
         <v>44</v>
       </c>
       <c r="F91" t="s">
-        <v>175</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="C92" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D92" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E92" t="s">
         <v>44</v>
       </c>
       <c r="F92" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
       <c r="C93" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D93" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E93" t="s">
         <v>44</v>
       </c>
       <c r="F93" t="s">
-        <v>252</v>
+        <v>145</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="C94" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D94" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E94" t="s">
         <v>44</v>
       </c>
       <c r="F94" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="C95" t="s">
         <v>195</v>
       </c>
       <c r="D95" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E95" t="s">
         <v>44</v>
       </c>
       <c r="F95" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="C96" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D96" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E96" t="s">
         <v>44</v>
       </c>
       <c r="F96" t="s">
-        <v>256</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="C97" t="s">
         <v>41</v>
@@ -4153,27 +4153,27 @@
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>259</v>
+        <v>273</v>
       </c>
       <c r="C98" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D98" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E98" t="s">
         <v>44</v>
       </c>
       <c r="F98" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>260</v>
+        <v>274</v>
       </c>
       <c r="C99" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D99" t="s">
         <v>43</v>
@@ -4182,83 +4182,83 @@
         <v>44</v>
       </c>
       <c r="F99" t="s">
-        <v>250</v>
+        <v>175</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>261</v>
+        <v>275</v>
       </c>
       <c r="C100" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D100" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E100" t="s">
         <v>44</v>
       </c>
       <c r="F100" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>262</v>
+        <v>276</v>
       </c>
       <c r="C101" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D101" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E101" t="s">
         <v>44</v>
       </c>
       <c r="F101" t="s">
-        <v>145</v>
+        <v>238</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>263</v>
+        <v>277</v>
       </c>
       <c r="C102" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D102" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E102" t="s">
         <v>44</v>
       </c>
       <c r="F102" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>264</v>
+        <v>278</v>
       </c>
       <c r="C103" t="s">
         <v>195</v>
       </c>
       <c r="D103" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E103" t="s">
         <v>44</v>
       </c>
       <c r="F103" t="s">
-        <v>205</v>
+        <v>145</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>265</v>
+        <v>279</v>
       </c>
       <c r="C104" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D104" t="s">
         <v>43</v>
@@ -4267,29 +4267,29 @@
         <v>44</v>
       </c>
       <c r="F104" t="s">
-        <v>145</v>
+        <v>258</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="C105" t="s">
         <v>41</v>
       </c>
       <c r="D105" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E105" t="s">
         <v>44</v>
       </c>
       <c r="F105" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="C106" t="s">
         <v>195</v>
@@ -4306,7 +4306,7 @@
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>274</v>
+        <v>282</v>
       </c>
       <c r="C107" t="s">
         <v>195</v>
@@ -4318,12 +4318,12 @@
         <v>44</v>
       </c>
       <c r="F107" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>275</v>
+        <v>283</v>
       </c>
       <c r="C108" t="s">
         <v>41</v>
@@ -4335,12 +4335,12 @@
         <v>44</v>
       </c>
       <c r="F108" t="s">
-        <v>250</v>
+        <v>258</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>276</v>
+        <v>284</v>
       </c>
       <c r="C109" t="s">
         <v>41</v>
@@ -4352,12 +4352,12 @@
         <v>44</v>
       </c>
       <c r="F109" t="s">
-        <v>238</v>
+        <v>244</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="C110" t="s">
         <v>195</v>
@@ -4374,7 +4374,7 @@
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C111" t="s">
         <v>195</v>
@@ -4391,7 +4391,7 @@
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="C112" t="s">
         <v>41</v>
@@ -4408,7 +4408,7 @@
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="C113" t="s">
         <v>41</v>
@@ -4420,12 +4420,12 @@
         <v>44</v>
       </c>
       <c r="F113" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="C114" t="s">
         <v>195</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="C115" t="s">
         <v>195</v>
@@ -4454,12 +4454,12 @@
         <v>44</v>
       </c>
       <c r="F115" t="s">
-        <v>145</v>
+        <v>175</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="C116" t="s">
         <v>41</v>
@@ -4471,12 +4471,12 @@
         <v>44</v>
       </c>
       <c r="F116" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>284</v>
+        <v>292</v>
       </c>
       <c r="C117" t="s">
         <v>41</v>
@@ -4488,12 +4488,12 @@
         <v>44</v>
       </c>
       <c r="F117" t="s">
-        <v>244</v>
+        <v>252</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>285</v>
+        <v>293</v>
       </c>
       <c r="C118" t="s">
         <v>195</v>
@@ -4510,7 +4510,7 @@
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>286</v>
+        <v>294</v>
       </c>
       <c r="C119" t="s">
         <v>195</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="C120" t="s">
         <v>41</v>
@@ -4544,7 +4544,7 @@
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>288</v>
+        <v>296</v>
       </c>
       <c r="C121" t="s">
         <v>41</v>
@@ -4556,12 +4556,12 @@
         <v>44</v>
       </c>
       <c r="F121" t="s">
-        <v>246</v>
+        <v>256</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>289</v>
+        <v>297</v>
       </c>
       <c r="C122" t="s">
         <v>195</v>
@@ -4578,7 +4578,7 @@
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>290</v>
+        <v>298</v>
       </c>
       <c r="C123" t="s">
         <v>195</v>
@@ -4590,12 +4590,12 @@
         <v>44</v>
       </c>
       <c r="F123" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>291</v>
+        <v>299</v>
       </c>
       <c r="C124" t="s">
         <v>41</v>
@@ -4607,12 +4607,12 @@
         <v>44</v>
       </c>
       <c r="F124" t="s">
-        <v>250</v>
+        <v>227</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
       <c r="C125" t="s">
         <v>41</v>
@@ -4624,12 +4624,12 @@
         <v>44</v>
       </c>
       <c r="F125" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C126" t="s">
         <v>195</v>
@@ -4646,7 +4646,7 @@
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>294</v>
+        <v>302</v>
       </c>
       <c r="C127" t="s">
         <v>195</v>
@@ -4658,12 +4658,12 @@
         <v>44</v>
       </c>
       <c r="F127" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="C128" t="s">
         <v>41</v>
@@ -4675,12 +4675,12 @@
         <v>44</v>
       </c>
       <c r="F128" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="C129" t="s">
         <v>41</v>
@@ -4692,12 +4692,12 @@
         <v>44</v>
       </c>
       <c r="F129" t="s">
-        <v>256</v>
+        <v>214</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>297</v>
+        <v>305</v>
       </c>
       <c r="C130" t="s">
         <v>195</v>
@@ -4714,7 +4714,7 @@
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="C131" t="s">
         <v>195</v>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="C132" t="s">
         <v>41</v>
@@ -4748,7 +4748,7 @@
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="C133" t="s">
         <v>41</v>
@@ -4760,18 +4760,18 @@
         <v>44</v>
       </c>
       <c r="F133" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="C134" t="s">
         <v>195</v>
       </c>
       <c r="D134" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E134" t="s">
         <v>44</v>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>302</v>
+        <v>310</v>
       </c>
       <c r="C135" t="s">
         <v>195</v>
@@ -4794,66 +4794,66 @@
         <v>44</v>
       </c>
       <c r="F135" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="C136" t="s">
         <v>41</v>
       </c>
       <c r="D136" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E136" t="s">
         <v>44</v>
       </c>
       <c r="F136" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>304</v>
+        <v>312</v>
       </c>
       <c r="C137" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D137" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E137" t="s">
         <v>44</v>
       </c>
       <c r="F137" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>305</v>
+        <v>313</v>
       </c>
       <c r="C138" t="s">
         <v>195</v>
       </c>
       <c r="D138" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E138" t="s">
         <v>44</v>
       </c>
       <c r="F138" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="C139" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D139" t="s">
         <v>43</v>
@@ -4862,32 +4862,32 @@
         <v>44</v>
       </c>
       <c r="F139" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>307</v>
+        <v>315</v>
       </c>
       <c r="C140" t="s">
         <v>41</v>
       </c>
       <c r="D140" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E140" t="s">
         <v>44</v>
       </c>
       <c r="F140" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>308</v>
+        <v>316</v>
       </c>
       <c r="C141" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D141" t="s">
         <v>73</v>
@@ -4896,49 +4896,49 @@
         <v>44</v>
       </c>
       <c r="F141" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>309</v>
+        <v>317</v>
       </c>
       <c r="C142" t="s">
         <v>195</v>
       </c>
       <c r="D142" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E142" t="s">
         <v>44</v>
       </c>
       <c r="F142" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>310</v>
+        <v>318</v>
       </c>
       <c r="C143" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D143" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E143" t="s">
         <v>44</v>
       </c>
       <c r="F143" t="s">
-        <v>223</v>
+        <v>208</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="C144" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D144" t="s">
         <v>73</v>
@@ -4947,32 +4947,32 @@
         <v>44</v>
       </c>
       <c r="F144" t="s">
-        <v>220</v>
+        <v>322</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>312</v>
+        <v>323</v>
       </c>
       <c r="C145" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D145" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E145" t="s">
         <v>44</v>
       </c>
       <c r="F145" t="s">
-        <v>205</v>
+        <v>153</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="C146" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D146" t="s">
         <v>43</v>
@@ -4981,12 +4981,12 @@
         <v>44</v>
       </c>
       <c r="F146" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="C147" t="s">
         <v>41</v>
@@ -4998,49 +4998,49 @@
         <v>44</v>
       </c>
       <c r="F147" t="s">
-        <v>232</v>
+        <v>150</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>315</v>
+        <v>326</v>
       </c>
       <c r="C148" t="s">
         <v>41</v>
       </c>
       <c r="D148" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E148" t="s">
         <v>44</v>
       </c>
       <c r="F148" t="s">
-        <v>210</v>
+        <v>145</v>
       </c>
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="C149" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D149" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E149" t="s">
         <v>44</v>
       </c>
       <c r="F149" t="s">
-        <v>205</v>
+        <v>147</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>317</v>
+        <v>328</v>
       </c>
       <c r="C150" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D150" t="s">
         <v>43</v>
@@ -5049,46 +5049,46 @@
         <v>44</v>
       </c>
       <c r="F150" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="C151" t="s">
         <v>41</v>
       </c>
       <c r="D151" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E151" t="s">
         <v>44</v>
       </c>
       <c r="F151" t="s">
-        <v>208</v>
+        <v>143</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
       <c r="C152" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D152" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E152" t="s">
         <v>44</v>
       </c>
       <c r="F152" t="s">
-        <v>322</v>
+        <v>145</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>323</v>
+        <v>331</v>
       </c>
       <c r="C153" t="s">
         <v>41</v>
@@ -5100,12 +5100,12 @@
         <v>44</v>
       </c>
       <c r="F153" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>324</v>
+        <v>332</v>
       </c>
       <c r="C154" t="s">
         <v>41</v>
@@ -5117,12 +5117,12 @@
         <v>44</v>
       </c>
       <c r="F154" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>325</v>
+        <v>333</v>
       </c>
       <c r="C155" t="s">
         <v>41</v>
@@ -5134,12 +5134,12 @@
         <v>44</v>
       </c>
       <c r="F155" t="s">
-        <v>150</v>
+        <v>345</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
       <c r="C156" t="s">
         <v>41</v>
@@ -5151,12 +5151,12 @@
         <v>44</v>
       </c>
       <c r="F156" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>327</v>
+        <v>337</v>
       </c>
       <c r="C157" t="s">
         <v>41</v>
@@ -5168,12 +5168,12 @@
         <v>44</v>
       </c>
       <c r="F157" t="s">
-        <v>147</v>
+        <v>346</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>328</v>
+        <v>339</v>
       </c>
       <c r="C158" t="s">
         <v>41</v>
@@ -5185,12 +5185,12 @@
         <v>44</v>
       </c>
       <c r="F158" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>329</v>
+        <v>341</v>
       </c>
       <c r="C159" t="s">
         <v>41</v>
@@ -5202,12 +5202,12 @@
         <v>44</v>
       </c>
       <c r="F159" t="s">
-        <v>143</v>
+        <v>347</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>330</v>
+        <v>343</v>
       </c>
       <c r="C160" t="s">
         <v>41</v>
@@ -5219,145 +5219,17 @@
         <v>44</v>
       </c>
       <c r="F160" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="B161" t="s">
-        <v>331</v>
-      </c>
-      <c r="C161" t="s">
-        <v>41</v>
-      </c>
-      <c r="D161" t="s">
-        <v>43</v>
-      </c>
-      <c r="E161" t="s">
-        <v>44</v>
-      </c>
-      <c r="F161" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="B162" t="s">
-        <v>332</v>
-      </c>
-      <c r="C162" t="s">
-        <v>41</v>
-      </c>
-      <c r="D162" t="s">
-        <v>43</v>
-      </c>
-      <c r="E162" t="s">
-        <v>44</v>
-      </c>
-      <c r="F162" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="B163" t="s">
-        <v>333</v>
-      </c>
-      <c r="C163" t="s">
-        <v>41</v>
-      </c>
-      <c r="D163" t="s">
-        <v>43</v>
-      </c>
-      <c r="E163" t="s">
-        <v>44</v>
-      </c>
-      <c r="F163" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="B164" t="s">
-        <v>335</v>
-      </c>
-      <c r="C164" t="s">
-        <v>41</v>
-      </c>
-      <c r="D164" t="s">
-        <v>43</v>
-      </c>
-      <c r="E164" t="s">
-        <v>44</v>
-      </c>
-      <c r="F164" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="165">
-      <c r="B165" t="s">
-        <v>337</v>
-      </c>
-      <c r="C165" t="s">
-        <v>41</v>
-      </c>
-      <c r="D165" t="s">
-        <v>43</v>
-      </c>
-      <c r="E165" t="s">
-        <v>44</v>
-      </c>
-      <c r="F165" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="B166" t="s">
-        <v>339</v>
-      </c>
-      <c r="C166" t="s">
-        <v>41</v>
-      </c>
-      <c r="D166" t="s">
-        <v>43</v>
-      </c>
-      <c r="E166" t="s">
-        <v>44</v>
-      </c>
-      <c r="F166" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="167">
-      <c r="B167" t="s">
-        <v>341</v>
-      </c>
-      <c r="C167" t="s">
-        <v>41</v>
-      </c>
-      <c r="D167" t="s">
-        <v>43</v>
-      </c>
-      <c r="E167" t="s">
-        <v>44</v>
-      </c>
-      <c r="F167" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="168">
-      <c r="B168" t="s">
-        <v>343</v>
-      </c>
-      <c r="C168" t="s">
-        <v>41</v>
-      </c>
-      <c r="D168" t="s">
-        <v>43</v>
-      </c>
-      <c r="E168" t="s">
-        <v>44</v>
-      </c>
-      <c r="F168" t="s">
-        <v>173</v>
-      </c>
-    </row>
+    <row r="161"/>
+    <row r="162"/>
+    <row r="163"/>
+    <row r="164"/>
+    <row r="165"/>
+    <row r="166"/>
+    <row r="167"/>
+    <row r="168"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added scale and lines connecting gpx points
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18995" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20941" uniqueCount="354">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1070,6 +1070,24 @@
   </si>
   <si>
     <t xml:space="preserve">Altitude: &lt;value&gt; m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId220</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;value&gt;&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId221</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100</t>
   </si>
 </sst>
 </file>
@@ -5222,9 +5240,57 @@
         <v>173</v>
       </c>
     </row>
-    <row r="161"/>
-    <row r="162"/>
-    <row r="163"/>
+    <row r="161">
+      <c r="B161" t="s">
+        <v>348</v>
+      </c>
+      <c r="C161" t="s">
+        <v>41</v>
+      </c>
+      <c r="D161" t="s">
+        <v>73</v>
+      </c>
+      <c r="E161" t="s">
+        <v>44</v>
+      </c>
+      <c r="F161" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="B162" t="s">
+        <v>351</v>
+      </c>
+      <c r="C162" t="s">
+        <v>41</v>
+      </c>
+      <c r="D162" t="s">
+        <v>43</v>
+      </c>
+      <c r="E162" t="s">
+        <v>44</v>
+      </c>
+      <c r="F162" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="B163" t="s">
+        <v>352</v>
+      </c>
+      <c r="C163" t="s">
+        <v>41</v>
+      </c>
+      <c r="D163" t="s">
+        <v>43</v>
+      </c>
+      <c r="E163" t="s">
+        <v>44</v>
+      </c>
+      <c r="F163" t="s">
+        <v>353</v>
+      </c>
+    </row>
     <row r="164"/>
     <row r="165"/>
     <row r="166"/>

</xml_diff>

<commit_message>
Added SdCard icon, removed unused screens
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20941" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22905" uniqueCount="358">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1088,6 +1088,18 @@
   </si>
   <si>
     <t xml:space="preserve">100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Path Tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId223</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId224</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logs</t>
   </si>
 </sst>
 </file>
@@ -3117,7 +3129,7 @@
     </row>
     <row r="36">
       <c r="B36" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C36" t="s">
         <v>38</v>
@@ -3129,29 +3141,29 @@
         <v>44</v>
       </c>
       <c r="F36" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C37" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E37" t="s">
         <v>44</v>
       </c>
       <c r="F37" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C38" t="s">
         <v>41</v>
@@ -3163,12 +3175,12 @@
         <v>44</v>
       </c>
       <c r="F38" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C39" t="s">
         <v>41</v>
@@ -3180,12 +3192,12 @@
         <v>44</v>
       </c>
       <c r="F39" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C40" t="s">
         <v>41</v>
@@ -3197,12 +3209,12 @@
         <v>44</v>
       </c>
       <c r="F40" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
@@ -3214,12 +3226,12 @@
         <v>44</v>
       </c>
       <c r="F41" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C42" t="s">
         <v>41</v>
@@ -3231,12 +3243,12 @@
         <v>44</v>
       </c>
       <c r="F42" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C43" t="s">
         <v>41</v>
@@ -3248,12 +3260,12 @@
         <v>44</v>
       </c>
       <c r="F43" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C44" t="s">
         <v>41</v>
@@ -3265,12 +3277,12 @@
         <v>44</v>
       </c>
       <c r="F44" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C45" t="s">
         <v>41</v>
@@ -3282,12 +3294,12 @@
         <v>44</v>
       </c>
       <c r="F45" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C46" t="s">
         <v>41</v>
@@ -3299,29 +3311,29 @@
         <v>44</v>
       </c>
       <c r="F46" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="s">
-        <v>154</v>
+        <v>181</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D47" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E47" t="s">
         <v>44</v>
       </c>
       <c r="F47" t="s">
-        <v>145</v>
+        <v>354</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="C48" t="s">
         <v>38</v>
@@ -3333,12 +3345,12 @@
         <v>44</v>
       </c>
       <c r="F48" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="C49" t="s">
         <v>38</v>
@@ -3350,46 +3362,46 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>182</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" t="s">
-        <v>183</v>
+        <v>199</v>
       </c>
       <c r="C50" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E50" t="s">
         <v>44</v>
       </c>
       <c r="F50" t="s">
-        <v>184</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C51" t="s">
-        <v>38</v>
+        <v>195</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E51" t="s">
         <v>44</v>
       </c>
       <c r="F51" t="s">
-        <v>197</v>
+        <v>173</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C52" t="s">
         <v>195</v>
@@ -3406,7 +3418,7 @@
     </row>
     <row r="53">
       <c r="B53" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="C53" t="s">
         <v>195</v>
@@ -3423,13 +3435,13 @@
     </row>
     <row r="54">
       <c r="B54" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="C54" t="s">
         <v>195</v>
       </c>
       <c r="D54" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E54" t="s">
         <v>44</v>
@@ -3440,7 +3452,7 @@
     </row>
     <row r="55">
       <c r="B55" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="C55" t="s">
         <v>195</v>
@@ -3452,15 +3464,15 @@
         <v>44</v>
       </c>
       <c r="F55" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
     </row>
     <row r="56">
       <c r="B56" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C56" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
         <v>73</v>
@@ -3469,29 +3481,29 @@
         <v>44</v>
       </c>
       <c r="F56" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57">
       <c r="B57" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="C57" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D57" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E57" t="s">
         <v>44</v>
       </c>
       <c r="F57" t="s">
-        <v>189</v>
+        <v>210</v>
       </c>
     </row>
     <row r="58">
       <c r="B58" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C58" t="s">
         <v>41</v>
@@ -3503,12 +3515,12 @@
         <v>44</v>
       </c>
       <c r="F58" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="59">
       <c r="B59" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C59" t="s">
         <v>41</v>
@@ -3520,12 +3532,12 @@
         <v>44</v>
       </c>
       <c r="F59" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
     </row>
     <row r="60">
       <c r="B60" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C60" t="s">
         <v>41</v>
@@ -3537,103 +3549,103 @@
         <v>44</v>
       </c>
       <c r="F60" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61">
       <c r="B61" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="C61" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D61" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E61" t="s">
         <v>44</v>
       </c>
       <c r="F61" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62">
       <c r="B62" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="C62" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E62" t="s">
         <v>44</v>
       </c>
       <c r="F62" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
     </row>
     <row r="63">
       <c r="B63" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D63" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E63" t="s">
         <v>44</v>
       </c>
       <c r="F63" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
     </row>
     <row r="64">
       <c r="B64" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="C64" t="s">
         <v>195</v>
       </c>
       <c r="D64" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E64" t="s">
         <v>44</v>
       </c>
       <c r="F64" t="s">
-        <v>173</v>
+        <v>205</v>
       </c>
     </row>
     <row r="65">
       <c r="B65" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="C65" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E65" t="s">
         <v>44</v>
       </c>
       <c r="F65" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66">
       <c r="B66" t="s">
-        <v>221</v>
+        <v>186</v>
       </c>
       <c r="C66" t="s">
         <v>195</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E66" t="s">
         <v>44</v>
@@ -3644,10 +3656,10 @@
     </row>
     <row r="67">
       <c r="B67" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="C67" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D67" t="s">
         <v>43</v>
@@ -3656,32 +3668,32 @@
         <v>44</v>
       </c>
       <c r="F67" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
     </row>
     <row r="68">
       <c r="B68" t="s">
-        <v>186</v>
+        <v>228</v>
       </c>
       <c r="C68" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E68" t="s">
         <v>44</v>
       </c>
       <c r="F68" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="69">
       <c r="B69" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C69" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D69" t="s">
         <v>43</v>
@@ -3690,12 +3702,12 @@
         <v>44</v>
       </c>
       <c r="F69" t="s">
-        <v>227</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70">
       <c r="B70" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C70" t="s">
         <v>41</v>
@@ -3712,10 +3724,10 @@
     </row>
     <row r="71">
       <c r="B71" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C71" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D71" t="s">
         <v>43</v>
@@ -3724,32 +3736,32 @@
         <v>44</v>
       </c>
       <c r="F71" t="s">
-        <v>173</v>
+        <v>232</v>
       </c>
     </row>
     <row r="72">
       <c r="B72" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C72" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D72" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E72" t="s">
         <v>44</v>
       </c>
       <c r="F72" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="C73" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D73" t="s">
         <v>43</v>
@@ -3758,97 +3770,97 @@
         <v>44</v>
       </c>
       <c r="F73" t="s">
-        <v>232</v>
+        <v>175</v>
       </c>
     </row>
     <row r="74">
       <c r="B74" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C74" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D74" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E74" t="s">
         <v>44</v>
       </c>
       <c r="F74" t="s">
-        <v>205</v>
+        <v>238</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C75" t="s">
         <v>195</v>
       </c>
       <c r="D75" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E75" t="s">
         <v>44</v>
       </c>
       <c r="F75" t="s">
-        <v>175</v>
+        <v>205</v>
       </c>
     </row>
     <row r="76">
       <c r="B76" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C76" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D76" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E76" t="s">
         <v>44</v>
       </c>
       <c r="F76" t="s">
-        <v>238</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C77" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D77" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E77" t="s">
         <v>44</v>
       </c>
       <c r="F77" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C78" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D78" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E78" t="s">
         <v>44</v>
       </c>
       <c r="F78" t="s">
-        <v>145</v>
+        <v>244</v>
       </c>
     </row>
     <row r="79">
       <c r="B79" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C79" t="s">
         <v>41</v>
@@ -3860,134 +3872,134 @@
         <v>44</v>
       </c>
       <c r="F79" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="80">
       <c r="B80" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="C80" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D80" t="s">
-        <v>73</v>
+        <v>225</v>
       </c>
       <c r="E80" t="s">
         <v>44</v>
       </c>
       <c r="F80" t="s">
-        <v>244</v>
+        <v>205</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C81" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D81" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E81" t="s">
         <v>44</v>
       </c>
       <c r="F81" t="s">
-        <v>246</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D82" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E82" t="s">
         <v>44</v>
       </c>
       <c r="F82" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
     </row>
     <row r="83">
       <c r="B83" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D83" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E83" t="s">
         <v>44</v>
       </c>
       <c r="F83" t="s">
-        <v>175</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C84" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D84" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E84" t="s">
         <v>44</v>
       </c>
       <c r="F84" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="C85" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D85" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E85" t="s">
         <v>44</v>
       </c>
       <c r="F85" t="s">
-        <v>252</v>
+        <v>145</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C86" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D86" t="s">
-        <v>225</v>
+        <v>73</v>
       </c>
       <c r="E86" t="s">
         <v>44</v>
       </c>
       <c r="F86" t="s">
-        <v>205</v>
+        <v>256</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C87" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D87" t="s">
         <v>43</v>
@@ -3996,29 +4008,29 @@
         <v>44</v>
       </c>
       <c r="F87" t="s">
-        <v>145</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
       <c r="C88" t="s">
         <v>41</v>
       </c>
       <c r="D88" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E88" t="s">
         <v>44</v>
       </c>
       <c r="F88" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="C89" t="s">
         <v>41</v>
@@ -4030,32 +4042,32 @@
         <v>44</v>
       </c>
       <c r="F89" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="C90" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D90" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E90" t="s">
         <v>44</v>
       </c>
       <c r="F90" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C91" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D91" t="s">
         <v>43</v>
@@ -4064,49 +4076,49 @@
         <v>44</v>
       </c>
       <c r="F91" t="s">
-        <v>250</v>
+        <v>145</v>
       </c>
     </row>
     <row r="92">
       <c r="B92" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="C92" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D92" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E92" t="s">
         <v>44</v>
       </c>
       <c r="F92" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="93">
       <c r="B93" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C93" t="s">
         <v>195</v>
       </c>
       <c r="D93" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E93" t="s">
         <v>44</v>
       </c>
       <c r="F93" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
     </row>
     <row r="94">
       <c r="B94" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C94" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D94" t="s">
         <v>43</v>
@@ -4115,49 +4127,49 @@
         <v>44</v>
       </c>
       <c r="F94" t="s">
-        <v>258</v>
+        <v>145</v>
       </c>
     </row>
     <row r="95">
       <c r="B95" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="C95" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D95" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E95" t="s">
         <v>44</v>
       </c>
       <c r="F95" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96">
       <c r="B96" t="s">
-        <v>265</v>
+        <v>273</v>
       </c>
       <c r="C96" t="s">
         <v>195</v>
       </c>
       <c r="D96" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E96" t="s">
         <v>44</v>
       </c>
       <c r="F96" t="s">
-        <v>145</v>
+        <v>205</v>
       </c>
     </row>
     <row r="97">
       <c r="B97" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C97" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D97" t="s">
         <v>43</v>
@@ -4166,627 +4178,627 @@
         <v>44</v>
       </c>
       <c r="F97" t="s">
-        <v>258</v>
+        <v>175</v>
       </c>
     </row>
     <row r="98">
       <c r="B98" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C98" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D98" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E98" t="s">
         <v>44</v>
       </c>
       <c r="F98" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
     </row>
     <row r="99">
       <c r="B99" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C99" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D99" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E99" t="s">
         <v>44</v>
       </c>
       <c r="F99" t="s">
-        <v>175</v>
+        <v>238</v>
       </c>
     </row>
     <row r="100">
       <c r="B100" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C100" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D100" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E100" t="s">
         <v>44</v>
       </c>
       <c r="F100" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101">
       <c r="B101" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="C101" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D101" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E101" t="s">
         <v>44</v>
       </c>
       <c r="F101" t="s">
-        <v>238</v>
+        <v>145</v>
       </c>
     </row>
     <row r="102">
       <c r="B102" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C102" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D102" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E102" t="s">
         <v>44</v>
       </c>
       <c r="F102" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="103">
       <c r="B103" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D103" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E103" t="s">
         <v>44</v>
       </c>
       <c r="F103" t="s">
-        <v>145</v>
+        <v>242</v>
       </c>
     </row>
     <row r="104">
       <c r="B104" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C104" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E104" t="s">
         <v>44</v>
       </c>
       <c r="F104" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="105">
       <c r="B105" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C105" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D105" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E105" t="s">
         <v>44</v>
       </c>
       <c r="F105" t="s">
-        <v>242</v>
+        <v>145</v>
       </c>
     </row>
     <row r="106">
       <c r="B106" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="C106" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D106" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E106" t="s">
         <v>44</v>
       </c>
       <c r="F106" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="107">
       <c r="B107" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="C107" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D107" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E107" t="s">
         <v>44</v>
       </c>
       <c r="F107" t="s">
-        <v>145</v>
+        <v>244</v>
       </c>
     </row>
     <row r="108">
       <c r="B108" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C108" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D108" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E108" t="s">
         <v>44</v>
       </c>
       <c r="F108" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="109">
       <c r="B109" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="C109" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D109" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E109" t="s">
         <v>44</v>
       </c>
       <c r="F109" t="s">
-        <v>244</v>
+        <v>145</v>
       </c>
     </row>
     <row r="110">
       <c r="B110" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="C110" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D110" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E110" t="s">
         <v>44</v>
       </c>
       <c r="F110" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="111">
       <c r="B111" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C111" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D111" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E111" t="s">
         <v>44</v>
       </c>
       <c r="F111" t="s">
-        <v>145</v>
+        <v>246</v>
       </c>
     </row>
     <row r="112">
       <c r="B112" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C112" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D112" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E112" t="s">
         <v>44</v>
       </c>
       <c r="F112" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="113">
       <c r="B113" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="C113" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D113" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E113" t="s">
         <v>44</v>
       </c>
       <c r="F113" t="s">
-        <v>246</v>
+        <v>175</v>
       </c>
     </row>
     <row r="114">
       <c r="B114" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C114" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D114" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E114" t="s">
         <v>44</v>
       </c>
       <c r="F114" t="s">
-        <v>205</v>
+        <v>250</v>
       </c>
     </row>
     <row r="115">
       <c r="B115" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="C115" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D115" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E115" t="s">
         <v>44</v>
       </c>
       <c r="F115" t="s">
-        <v>175</v>
+        <v>252</v>
       </c>
     </row>
     <row r="116">
       <c r="B116" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="C116" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D116" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E116" t="s">
         <v>44</v>
       </c>
       <c r="F116" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
     </row>
     <row r="117">
       <c r="B117" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="C117" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D117" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E117" t="s">
         <v>44</v>
       </c>
       <c r="F117" t="s">
-        <v>252</v>
+        <v>145</v>
       </c>
     </row>
     <row r="118">
       <c r="B118" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C118" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D118" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E118" t="s">
         <v>44</v>
       </c>
       <c r="F118" t="s">
-        <v>205</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119">
       <c r="B119" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C119" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D119" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E119" t="s">
         <v>44</v>
       </c>
       <c r="F119" t="s">
-        <v>145</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120">
       <c r="B120" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="C120" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D120" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E120" t="s">
         <v>44</v>
       </c>
       <c r="F120" t="s">
-        <v>258</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121">
       <c r="B121" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="C121" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D121" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E121" t="s">
         <v>44</v>
       </c>
       <c r="F121" t="s">
-        <v>256</v>
+        <v>173</v>
       </c>
     </row>
     <row r="122">
       <c r="B122" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="C122" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D122" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E122" t="s">
         <v>44</v>
       </c>
       <c r="F122" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="123">
       <c r="B123" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C123" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D123" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E123" t="s">
         <v>44</v>
       </c>
       <c r="F123" t="s">
-        <v>173</v>
+        <v>216</v>
       </c>
     </row>
     <row r="124">
       <c r="B124" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="C124" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D124" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E124" t="s">
         <v>44</v>
       </c>
       <c r="F124" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="125">
       <c r="B125" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="C125" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D125" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E125" t="s">
         <v>44</v>
       </c>
       <c r="F125" t="s">
-        <v>216</v>
+        <v>173</v>
       </c>
     </row>
     <row r="126">
       <c r="B126" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="C126" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D126" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E126" t="s">
         <v>44</v>
       </c>
       <c r="F126" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="127">
       <c r="B127" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="C127" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D127" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E127" t="s">
         <v>44</v>
       </c>
       <c r="F127" t="s">
-        <v>173</v>
+        <v>214</v>
       </c>
     </row>
     <row r="128">
       <c r="B128" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C128" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D128" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E128" t="s">
         <v>44</v>
       </c>
       <c r="F128" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="129">
       <c r="B129" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="C129" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D129" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E129" t="s">
         <v>44</v>
       </c>
       <c r="F129" t="s">
-        <v>214</v>
+        <v>173</v>
       </c>
     </row>
     <row r="130">
       <c r="B130" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="C130" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D130" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E130" t="s">
         <v>44</v>
       </c>
       <c r="F130" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
     </row>
     <row r="131">
       <c r="B131" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C131" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D131" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E131" t="s">
         <v>44</v>
       </c>
       <c r="F131" t="s">
-        <v>173</v>
+        <v>212</v>
       </c>
     </row>
     <row r="132">
       <c r="B132" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C132" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D132" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E132" t="s">
         <v>44</v>
       </c>
       <c r="F132" t="s">
-        <v>227</v>
+        <v>205</v>
       </c>
     </row>
     <row r="133">
       <c r="B133" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C133" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D133" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E133" t="s">
         <v>44</v>
       </c>
       <c r="F133" t="s">
-        <v>212</v>
+        <v>223</v>
       </c>
     </row>
     <row r="134">
       <c r="B134" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="C134" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D134" t="s">
         <v>73</v>
@@ -4795,117 +4807,117 @@
         <v>44</v>
       </c>
       <c r="F134" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
     </row>
     <row r="135">
       <c r="B135" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C135" t="s">
         <v>195</v>
       </c>
       <c r="D135" t="s">
-        <v>43</v>
+        <v>225</v>
       </c>
       <c r="E135" t="s">
         <v>44</v>
       </c>
       <c r="F135" t="s">
-        <v>223</v>
+        <v>205</v>
       </c>
     </row>
     <row r="136">
       <c r="B136" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C136" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D136" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E136" t="s">
         <v>44</v>
       </c>
       <c r="F136" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
     </row>
     <row r="137">
       <c r="B137" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="C137" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D137" t="s">
-        <v>225</v>
+        <v>43</v>
       </c>
       <c r="E137" t="s">
         <v>44</v>
       </c>
       <c r="F137" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
     </row>
     <row r="138">
       <c r="B138" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="C138" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D138" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E138" t="s">
         <v>44</v>
       </c>
       <c r="F138" t="s">
-        <v>173</v>
+        <v>210</v>
       </c>
     </row>
     <row r="139">
       <c r="B139" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C139" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D139" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E139" t="s">
         <v>44</v>
       </c>
       <c r="F139" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
     </row>
     <row r="140">
       <c r="B140" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C140" t="s">
-        <v>41</v>
+        <v>195</v>
       </c>
       <c r="D140" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E140" t="s">
         <v>44</v>
       </c>
       <c r="F140" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
     </row>
     <row r="141">
       <c r="B141" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="C141" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="D141" t="s">
         <v>73</v>
@@ -4914,63 +4926,63 @@
         <v>44</v>
       </c>
       <c r="F141" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
     </row>
     <row r="142">
       <c r="B142" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="C142" t="s">
-        <v>195</v>
+        <v>38</v>
       </c>
       <c r="D142" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E142" t="s">
         <v>44</v>
       </c>
       <c r="F142" t="s">
-        <v>189</v>
+        <v>322</v>
       </c>
     </row>
     <row r="143">
       <c r="B143" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C143" t="s">
         <v>41</v>
       </c>
       <c r="D143" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E143" t="s">
         <v>44</v>
       </c>
       <c r="F143" t="s">
-        <v>208</v>
+        <v>153</v>
       </c>
     </row>
     <row r="144">
       <c r="B144" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="C144" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D144" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E144" t="s">
         <v>44</v>
       </c>
       <c r="F144" t="s">
-        <v>322</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145">
       <c r="B145" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="C145" t="s">
         <v>41</v>
@@ -4982,12 +4994,12 @@
         <v>44</v>
       </c>
       <c r="F145" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="146">
       <c r="B146" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C146" t="s">
         <v>41</v>
@@ -5004,7 +5016,7 @@
     </row>
     <row r="147">
       <c r="B147" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C147" t="s">
         <v>41</v>
@@ -5016,12 +5028,12 @@
         <v>44</v>
       </c>
       <c r="F147" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="148">
       <c r="B148" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C148" t="s">
         <v>41</v>
@@ -5038,7 +5050,7 @@
     </row>
     <row r="149">
       <c r="B149" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C149" t="s">
         <v>41</v>
@@ -5050,12 +5062,12 @@
         <v>44</v>
       </c>
       <c r="F149" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="150">
       <c r="B150" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C150" t="s">
         <v>41</v>
@@ -5072,7 +5084,7 @@
     </row>
     <row r="151">
       <c r="B151" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C151" t="s">
         <v>41</v>
@@ -5084,12 +5096,12 @@
         <v>44</v>
       </c>
       <c r="F151" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="152">
       <c r="B152" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C152" t="s">
         <v>41</v>
@@ -5101,12 +5113,12 @@
         <v>44</v>
       </c>
       <c r="F152" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="153">
       <c r="B153" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="C153" t="s">
         <v>41</v>
@@ -5118,12 +5130,12 @@
         <v>44</v>
       </c>
       <c r="F153" t="s">
-        <v>139</v>
+        <v>345</v>
       </c>
     </row>
     <row r="154">
       <c r="B154" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="C154" t="s">
         <v>41</v>
@@ -5135,12 +5147,12 @@
         <v>44</v>
       </c>
       <c r="F154" t="s">
-        <v>141</v>
+        <v>173</v>
       </c>
     </row>
     <row r="155">
       <c r="B155" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="C155" t="s">
         <v>41</v>
@@ -5152,12 +5164,12 @@
         <v>44</v>
       </c>
       <c r="F155" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="156">
       <c r="B156" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="C156" t="s">
         <v>41</v>
@@ -5174,7 +5186,7 @@
     </row>
     <row r="157">
       <c r="B157" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="C157" t="s">
         <v>41</v>
@@ -5186,12 +5198,12 @@
         <v>44</v>
       </c>
       <c r="F157" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="158">
       <c r="B158" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="C158" t="s">
         <v>41</v>
@@ -5208,24 +5220,24 @@
     </row>
     <row r="159">
       <c r="B159" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="C159" t="s">
         <v>41</v>
       </c>
       <c r="D159" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E159" t="s">
         <v>44</v>
       </c>
       <c r="F159" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
     </row>
     <row r="160">
       <c r="B160" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="C160" t="s">
         <v>41</v>
@@ -5237,58 +5249,58 @@
         <v>44</v>
       </c>
       <c r="F160" t="s">
-        <v>173</v>
+        <v>258</v>
       </c>
     </row>
     <row r="161">
       <c r="B161" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="C161" t="s">
         <v>41</v>
       </c>
       <c r="D161" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E161" t="s">
         <v>44</v>
       </c>
       <c r="F161" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
     </row>
     <row r="162">
       <c r="B162" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C162" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D162" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E162" t="s">
         <v>44</v>
       </c>
       <c r="F162" t="s">
-        <v>258</v>
+        <v>180</v>
       </c>
     </row>
     <row r="163">
       <c r="B163" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="C163" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="D163" t="s">
-        <v>43</v>
+        <v>73</v>
       </c>
       <c r="E163" t="s">
         <v>44</v>
       </c>
       <c r="F163" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
     </row>
     <row r="164"/>

</xml_diff>

<commit_message>
Activated alti sensor, added timezone in date
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22905" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30238" uniqueCount="380">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1100,6 +1100,72 @@
   </si>
   <si>
     <t xml:space="preserve">Logs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId225</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId226</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId227</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId229</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId230</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId231</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId232</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId233</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId234</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId235</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId236</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Element</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId237</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId238</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Var name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId239</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId240</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId241</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId242</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId243</t>
   </si>
 </sst>
 </file>
@@ -5303,11 +5369,265 @@
         <v>357</v>
       </c>
     </row>
-    <row r="164"/>
-    <row r="165"/>
-    <row r="166"/>
-    <row r="167"/>
-    <row r="168"/>
+    <row r="164">
+      <c r="B164" t="s">
+        <v>358</v>
+      </c>
+      <c r="C164" t="s">
+        <v>38</v>
+      </c>
+      <c r="D164" t="s">
+        <v>73</v>
+      </c>
+      <c r="E164" t="s">
+        <v>44</v>
+      </c>
+      <c r="F164" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="B165" t="s">
+        <v>359</v>
+      </c>
+      <c r="C165" t="s">
+        <v>38</v>
+      </c>
+      <c r="D165" t="s">
+        <v>43</v>
+      </c>
+      <c r="E165" t="s">
+        <v>44</v>
+      </c>
+      <c r="F165" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="B166" t="s">
+        <v>360</v>
+      </c>
+      <c r="C166" t="s">
+        <v>38</v>
+      </c>
+      <c r="D166" t="s">
+        <v>43</v>
+      </c>
+      <c r="E166" t="s">
+        <v>44</v>
+      </c>
+      <c r="F166" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="B167" t="s">
+        <v>361</v>
+      </c>
+      <c r="C167" t="s">
+        <v>38</v>
+      </c>
+      <c r="D167" t="s">
+        <v>43</v>
+      </c>
+      <c r="E167" t="s">
+        <v>44</v>
+      </c>
+      <c r="F167" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="B168" t="s">
+        <v>362</v>
+      </c>
+      <c r="C168" t="s">
+        <v>38</v>
+      </c>
+      <c r="D168" t="s">
+        <v>43</v>
+      </c>
+      <c r="E168" t="s">
+        <v>44</v>
+      </c>
+      <c r="F168" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="B169" t="s">
+        <v>363</v>
+      </c>
+      <c r="C169" t="s">
+        <v>38</v>
+      </c>
+      <c r="D169" t="s">
+        <v>43</v>
+      </c>
+      <c r="E169" t="s">
+        <v>44</v>
+      </c>
+      <c r="F169" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="B170" t="s">
+        <v>364</v>
+      </c>
+      <c r="C170" t="s">
+        <v>38</v>
+      </c>
+      <c r="D170" t="s">
+        <v>43</v>
+      </c>
+      <c r="E170" t="s">
+        <v>44</v>
+      </c>
+      <c r="F170" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="B171" t="s">
+        <v>365</v>
+      </c>
+      <c r="C171" t="s">
+        <v>38</v>
+      </c>
+      <c r="D171" t="s">
+        <v>43</v>
+      </c>
+      <c r="E171" t="s">
+        <v>44</v>
+      </c>
+      <c r="F171" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="B172" t="s">
+        <v>366</v>
+      </c>
+      <c r="C172" t="s">
+        <v>38</v>
+      </c>
+      <c r="D172" t="s">
+        <v>43</v>
+      </c>
+      <c r="E172" t="s">
+        <v>44</v>
+      </c>
+      <c r="F172" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="B173" t="s">
+        <v>367</v>
+      </c>
+      <c r="C173" t="s">
+        <v>38</v>
+      </c>
+      <c r="D173" t="s">
+        <v>43</v>
+      </c>
+      <c r="E173" t="s">
+        <v>44</v>
+      </c>
+      <c r="F173" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="B174" t="s">
+        <v>368</v>
+      </c>
+      <c r="C174" t="s">
+        <v>38</v>
+      </c>
+      <c r="D174" t="s">
+        <v>43</v>
+      </c>
+      <c r="E174" t="s">
+        <v>44</v>
+      </c>
+      <c r="F174" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="B175" t="s">
+        <v>369</v>
+      </c>
+      <c r="C175" t="s">
+        <v>41</v>
+      </c>
+      <c r="D175" t="s">
+        <v>73</v>
+      </c>
+      <c r="E175" t="s">
+        <v>44</v>
+      </c>
+      <c r="F175" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="B176" t="s">
+        <v>371</v>
+      </c>
+      <c r="C176" t="s">
+        <v>195</v>
+      </c>
+      <c r="D176" t="s">
+        <v>73</v>
+      </c>
+      <c r="E176" t="s">
+        <v>44</v>
+      </c>
+      <c r="F176" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="B177" t="s">
+        <v>372</v>
+      </c>
+      <c r="C177" t="s">
+        <v>38</v>
+      </c>
+      <c r="D177" t="s">
+        <v>43</v>
+      </c>
+      <c r="E177" t="s">
+        <v>44</v>
+      </c>
+      <c r="F177" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="B178" t="s">
+        <v>374</v>
+      </c>
+      <c r="C178" t="s">
+        <v>195</v>
+      </c>
+      <c r="D178" t="s">
+        <v>43</v>
+      </c>
+      <c r="E178" t="s">
+        <v>44</v>
+      </c>
+      <c r="F178" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="179"/>
+    <row r="180"/>
+    <row r="181"/>
+    <row r="182"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Added select screen, improved sensors enabling
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30238" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32400" uniqueCount="385">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1166,6 +1166,21 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId243</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21.3 km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     &lt;value&gt; km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31.3</t>
   </si>
 </sst>
 </file>
@@ -5624,8 +5639,40 @@
         <v>375</v>
       </c>
     </row>
-    <row r="179"/>
-    <row r="180"/>
+    <row r="179">
+      <c r="B179" t="s">
+        <v>380</v>
+      </c>
+      <c r="C179" t="s">
+        <v>38</v>
+      </c>
+      <c r="D179" t="s">
+        <v>73</v>
+      </c>
+      <c r="E179" t="s">
+        <v>44</v>
+      </c>
+      <c r="F179" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="B180" t="s">
+        <v>381</v>
+      </c>
+      <c r="C180" t="s">
+        <v>38</v>
+      </c>
+      <c r="D180" t="s">
+        <v>43</v>
+      </c>
+      <c r="E180" t="s">
+        <v>44</v>
+      </c>
+      <c r="F180" t="s">
+        <v>384</v>
+      </c>
+    </row>
     <row r="181"/>
     <row r="182"/>
   </sheetData>

</xml_diff>

<commit_message>
Added map selector menu
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32400" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40018" uniqueCount="388">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -1181,6 +1181,15 @@
   </si>
   <si>
     <t xml:space="preserve">31.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId261</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x41-0x7A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x20-0x7F</t>
   </si>
 </sst>
 </file>
@@ -2424,7 +2433,9 @@
       </c>
       <c r="G4"/>
       <c r="H4"/>
-      <c r="I4"/>
+      <c r="I4" t="s">
+        <v>387</v>
+      </c>
       <c r="J4"/>
       <c r="L4" s="4" t="s">
         <v>9</v>
@@ -2460,7 +2471,9 @@
       </c>
       <c r="G5"/>
       <c r="H5"/>
-      <c r="I5"/>
+      <c r="I5" t="s">
+        <v>387</v>
+      </c>
       <c r="J5"/>
       <c r="L5" s="7" t="s">
         <v>1</v>
@@ -2495,7 +2508,7 @@
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6" t="s">
-        <v>54</v>
+        <v>387</v>
       </c>
       <c r="J6"/>
       <c r="L6" s="7" t="s">
@@ -2531,7 +2544,7 @@
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>387</v>
       </c>
       <c r="J7"/>
       <c r="L7" s="7" t="s">
@@ -3443,7 +3456,7 @@
         <v>44</v>
       </c>
       <c r="F49" t="s">
-        <v>197</v>
+        <v>205</v>
       </c>
     </row>
     <row r="50">
@@ -5647,13 +5660,13 @@
         <v>38</v>
       </c>
       <c r="D179" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E179" t="s">
         <v>44</v>
       </c>
       <c r="F179" t="s">
-        <v>383</v>
+        <v>202</v>
       </c>
     </row>
     <row r="180">
@@ -5673,7 +5686,23 @@
         <v>384</v>
       </c>
     </row>
-    <row r="181"/>
+    <row r="181">
+      <c r="B181" t="s">
+        <v>385</v>
+      </c>
+      <c r="C181" t="s">
+        <v>38</v>
+      </c>
+      <c r="D181" t="s">
+        <v>43</v>
+      </c>
+      <c r="E181" t="s">
+        <v>44</v>
+      </c>
+      <c r="F181" t="s">
+        <v>197</v>
+      </c>
+    </row>
     <row r="182"/>
   </sheetData>
   <mergeCells count="1">

</xml_diff>